<commit_message>
Added family members management feature, including the ability to add, edit, and delete family members. Updated UI to support family-related functionalities and integrated family member selection in expense forms. Also updated translations and settings for new features.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Templates" sheetId="8" r:id="rId8"/>
     <sheet name="Accounts" sheetId="9" r:id="rId9"/>
     <sheet name="Transfers" sheetId="10" r:id="rId10"/>
+    <sheet name="FamilyMembers" sheetId="11" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
@@ -1456,6 +1457,36 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>relation</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Husna</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Sister</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I257"/>

</xml_diff>

<commit_message>
Refactored family member input handling in index.html to improve code readability and maintainability. Updated logic to safely access input values, ensuring no errors occur if elements are missing. Updated finance_data.xlsx file.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -408,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,18 +430,21 @@
         <v>account</v>
       </c>
       <c r="F1" t="str">
+        <v>familyMember</v>
+      </c>
+      <c r="G1" t="str">
         <v>notes</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>recurring</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>recurringFrequency</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>recurringNextDate</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>paymentMethod</v>
       </c>
     </row>
@@ -461,14 +464,11 @@
       <c r="E2" t="str">
         <v>Hand Cash</v>
       </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="str">
-        <v/>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
       </c>
       <c r="I2" t="str">
         <v/>
@@ -493,19 +493,19 @@
       <c r="E3" t="str">
         <v>Dutch Bangla Bank</v>
       </c>
-      <c r="F3" t="str">
-        <v/>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="str">
-        <v/>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
       </c>
       <c r="I3" t="str">
         <v/>
       </c>
       <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
         <v/>
       </c>
     </row>
@@ -525,19 +525,19 @@
       <c r="E4" t="str">
         <v/>
       </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="str">
-        <v/>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
       </c>
       <c r="I4" t="str">
         <v/>
       </c>
       <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
         <v/>
       </c>
     </row>
@@ -557,19 +557,19 @@
       <c r="E5" t="str">
         <v/>
       </c>
-      <c r="F5" t="str">
-        <v/>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <v/>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
       </c>
       <c r="I5" t="str">
         <v/>
       </c>
       <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
         <v/>
       </c>
     </row>
@@ -589,19 +589,19 @@
       <c r="E6" t="str">
         <v/>
       </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="str">
-        <v/>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
       </c>
       <c r="I6" t="str">
         <v/>
       </c>
       <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
         <v/>
       </c>
     </row>
@@ -621,19 +621,19 @@
       <c r="E7" t="str">
         <v/>
       </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="str">
-        <v/>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
       </c>
       <c r="I7" t="str">
         <v/>
       </c>
       <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
         <v/>
       </c>
     </row>
@@ -653,19 +653,19 @@
       <c r="E8" t="str">
         <v/>
       </c>
-      <c r="F8" t="str">
-        <v/>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="str">
-        <v/>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <v/>
       </c>
       <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
         <v/>
       </c>
     </row>
@@ -685,19 +685,19 @@
       <c r="E9" t="str">
         <v/>
       </c>
-      <c r="F9" t="str">
-        <v/>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="str">
-        <v/>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
       </c>
       <c r="I9" t="str">
         <v/>
       </c>
       <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
         <v/>
       </c>
     </row>
@@ -717,19 +717,19 @@
       <c r="E10" t="str">
         <v/>
       </c>
-      <c r="F10" t="str">
-        <v/>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="str">
-        <v/>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
       </c>
       <c r="I10" t="str">
         <v/>
       </c>
       <c r="J10" t="str">
+        <v/>
+      </c>
+      <c r="K10" t="str">
         <v/>
       </c>
     </row>
@@ -749,19 +749,19 @@
       <c r="E11" t="str">
         <v/>
       </c>
-      <c r="F11" t="str">
-        <v/>
-      </c>
-      <c r="G11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="str">
-        <v/>
+      <c r="G11" t="str">
+        <v/>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
       </c>
       <c r="I11" t="str">
         <v/>
       </c>
       <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
         <v/>
       </c>
     </row>
@@ -781,19 +781,19 @@
       <c r="E12" t="str">
         <v/>
       </c>
-      <c r="F12" t="str">
-        <v/>
-      </c>
-      <c r="G12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="str">
-        <v/>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
       </c>
       <c r="I12" t="str">
         <v/>
       </c>
       <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12" t="str">
         <v/>
       </c>
     </row>
@@ -813,19 +813,19 @@
       <c r="E13" t="str">
         <v/>
       </c>
-      <c r="F13" t="str">
-        <v/>
-      </c>
-      <c r="G13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H13" t="str">
-        <v/>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
       </c>
       <c r="I13" t="str">
         <v/>
       </c>
       <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
         <v/>
       </c>
     </row>
@@ -845,19 +845,19 @@
       <c r="E14" t="str">
         <v/>
       </c>
-      <c r="F14" t="str">
-        <v/>
-      </c>
-      <c r="G14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" t="str">
-        <v/>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
       </c>
       <c r="I14" t="str">
         <v/>
       </c>
       <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
         <v/>
       </c>
     </row>
@@ -877,19 +877,19 @@
       <c r="E15" t="str">
         <v/>
       </c>
-      <c r="F15" t="str">
-        <v/>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="str">
-        <v/>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
       </c>
       <c r="I15" t="str">
         <v/>
       </c>
       <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
         <v/>
       </c>
     </row>
@@ -909,19 +909,19 @@
       <c r="E16" t="str">
         <v/>
       </c>
-      <c r="F16" t="str">
-        <v/>
-      </c>
-      <c r="G16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="str">
-        <v/>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
       </c>
       <c r="I16" t="str">
         <v/>
       </c>
       <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
         <v/>
       </c>
     </row>
@@ -941,19 +941,19 @@
       <c r="E17" t="str">
         <v/>
       </c>
-      <c r="F17" t="str">
-        <v/>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="str">
-        <v/>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
       </c>
       <c r="I17" t="str">
         <v/>
       </c>
       <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17" t="str">
         <v/>
       </c>
     </row>
@@ -973,19 +973,19 @@
       <c r="E18" t="str">
         <v/>
       </c>
-      <c r="F18" t="str">
-        <v/>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="str">
-        <v/>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
       </c>
       <c r="I18" t="str">
         <v/>
       </c>
       <c r="J18" t="str">
+        <v/>
+      </c>
+      <c r="K18" t="str">
         <v/>
       </c>
     </row>
@@ -1005,19 +1005,19 @@
       <c r="E19" t="str">
         <v/>
       </c>
-      <c r="F19" t="str">
-        <v/>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="str">
-        <v/>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
       </c>
       <c r="I19" t="str">
         <v/>
       </c>
       <c r="J19" t="str">
+        <v/>
+      </c>
+      <c r="K19" t="str">
         <v/>
       </c>
     </row>
@@ -1037,19 +1037,19 @@
       <c r="E20" t="str">
         <v/>
       </c>
-      <c r="F20" t="str">
-        <v/>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" t="str">
-        <v/>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
       </c>
       <c r="I20" t="str">
         <v/>
       </c>
       <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20" t="str">
         <v/>
       </c>
     </row>
@@ -1069,19 +1069,19 @@
       <c r="E21" t="str">
         <v/>
       </c>
-      <c r="F21" t="str">
-        <v/>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" t="str">
-        <v/>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
       </c>
       <c r="I21" t="str">
         <v/>
       </c>
       <c r="J21" t="str">
+        <v/>
+      </c>
+      <c r="K21" t="str">
         <v/>
       </c>
     </row>
@@ -1101,19 +1101,19 @@
       <c r="E22" t="str">
         <v/>
       </c>
-      <c r="F22" t="str">
-        <v/>
-      </c>
-      <c r="G22" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" t="str">
-        <v/>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
       </c>
       <c r="I22" t="str">
         <v/>
       </c>
       <c r="J22" t="str">
+        <v/>
+      </c>
+      <c r="K22" t="str">
         <v/>
       </c>
     </row>
@@ -1133,19 +1133,19 @@
       <c r="E23" t="str">
         <v/>
       </c>
-      <c r="F23" t="str">
-        <v/>
-      </c>
-      <c r="G23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" t="str">
-        <v/>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
       </c>
       <c r="I23" t="str">
         <v/>
       </c>
       <c r="J23" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
         <v/>
       </c>
     </row>
@@ -1165,19 +1165,19 @@
       <c r="E24" t="str">
         <v/>
       </c>
-      <c r="F24" t="str">
-        <v/>
-      </c>
-      <c r="G24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" t="str">
-        <v/>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
       </c>
       <c r="I24" t="str">
         <v/>
       </c>
       <c r="J24" t="str">
+        <v/>
+      </c>
+      <c r="K24" t="str">
         <v/>
       </c>
     </row>
@@ -1197,19 +1197,19 @@
       <c r="E25" t="str">
         <v/>
       </c>
-      <c r="F25" t="str">
-        <v/>
-      </c>
-      <c r="G25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" t="str">
-        <v/>
+      <c r="G25" t="str">
+        <v/>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
       </c>
       <c r="I25" t="str">
         <v/>
       </c>
       <c r="J25" t="str">
+        <v/>
+      </c>
+      <c r="K25" t="str">
         <v/>
       </c>
     </row>
@@ -1229,19 +1229,19 @@
       <c r="E26" t="str">
         <v/>
       </c>
-      <c r="F26" t="str">
-        <v/>
-      </c>
-      <c r="G26" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" t="str">
-        <v/>
+      <c r="G26" t="str">
+        <v/>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
       </c>
       <c r="I26" t="str">
         <v/>
       </c>
       <c r="J26" t="str">
+        <v/>
+      </c>
+      <c r="K26" t="str">
         <v/>
       </c>
     </row>
@@ -1261,19 +1261,19 @@
       <c r="E27" t="str">
         <v/>
       </c>
-      <c r="F27" t="str">
-        <v/>
-      </c>
-      <c r="G27" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" t="str">
-        <v/>
+      <c r="G27" t="str">
+        <v/>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
       </c>
       <c r="I27" t="str">
         <v/>
       </c>
       <c r="J27" t="str">
+        <v/>
+      </c>
+      <c r="K27" t="str">
         <v/>
       </c>
     </row>
@@ -1293,19 +1293,19 @@
       <c r="E28" t="str">
         <v/>
       </c>
-      <c r="F28" t="str">
-        <v/>
-      </c>
-      <c r="G28" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" t="str">
-        <v/>
+      <c r="G28" t="str">
+        <v/>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
       </c>
       <c r="I28" t="str">
         <v/>
       </c>
       <c r="J28" t="str">
+        <v/>
+      </c>
+      <c r="K28" t="str">
         <v/>
       </c>
     </row>
@@ -1325,19 +1325,19 @@
       <c r="E29" t="str">
         <v/>
       </c>
-      <c r="F29" t="str">
-        <v/>
-      </c>
-      <c r="G29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" t="str">
-        <v/>
+      <c r="G29" t="str">
+        <v/>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
       </c>
       <c r="I29" t="str">
         <v/>
       </c>
       <c r="J29" t="str">
+        <v/>
+      </c>
+      <c r="K29" t="str">
         <v/>
       </c>
     </row>
@@ -1357,19 +1357,19 @@
       <c r="E30" t="str">
         <v/>
       </c>
-      <c r="F30" t="str">
-        <v/>
-      </c>
-      <c r="G30" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" t="str">
-        <v/>
+      <c r="G30" t="str">
+        <v/>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
       </c>
       <c r="I30" t="str">
         <v/>
       </c>
       <c r="J30" t="str">
+        <v/>
+      </c>
+      <c r="K30" t="str">
         <v/>
       </c>
     </row>
@@ -1389,19 +1389,19 @@
       <c r="E31" t="str">
         <v/>
       </c>
-      <c r="F31" t="str">
-        <v/>
-      </c>
-      <c r="G31" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" t="str">
-        <v/>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
       </c>
       <c r="I31" t="str">
         <v/>
       </c>
       <c r="J31" t="str">
+        <v/>
+      </c>
+      <c r="K31" t="str">
         <v/>
       </c>
     </row>
@@ -1421,25 +1421,25 @@
       <c r="E32" t="str">
         <v/>
       </c>
-      <c r="F32" t="str">
-        <v/>
-      </c>
-      <c r="G32" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" t="str">
-        <v/>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
       </c>
       <c r="I32" t="str">
         <v/>
       </c>
       <c r="J32" t="str">
+        <v/>
+      </c>
+      <c r="K32" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J32"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K32"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1542,6 +1542,9 @@
       <c r="E2" t="str">
         <v>Hand Cash</v>
       </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
       <c r="G2" t="str">
         <v/>
       </c>
@@ -1571,6 +1574,9 @@
       <c r="E3" t="str">
         <v/>
       </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
       <c r="G3" t="str">
         <v/>
       </c>
@@ -1600,6 +1606,9 @@
       <c r="E4" t="str">
         <v/>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
       <c r="G4" t="str">
         <v/>
       </c>
@@ -1629,6 +1638,9 @@
       <c r="E5" t="str">
         <v/>
       </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
       <c r="G5" t="str">
         <v/>
       </c>
@@ -1658,6 +1670,9 @@
       <c r="E6" t="str">
         <v/>
       </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
       <c r="G6" t="str">
         <v/>
       </c>
@@ -1687,6 +1702,9 @@
       <c r="E7" t="str">
         <v/>
       </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
       <c r="G7" t="str">
         <v/>
       </c>
@@ -1716,6 +1734,9 @@
       <c r="E8" t="str">
         <v/>
       </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
       <c r="G8" t="str">
         <v/>
       </c>
@@ -1745,6 +1766,9 @@
       <c r="E9" t="str">
         <v/>
       </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
       <c r="G9" t="str">
         <v/>
       </c>
@@ -1774,6 +1798,9 @@
       <c r="E10" t="str">
         <v/>
       </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
       <c r="G10" t="str">
         <v/>
       </c>
@@ -1803,6 +1830,9 @@
       <c r="E11" t="str">
         <v/>
       </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
       <c r="G11" t="str">
         <v/>
       </c>
@@ -1832,6 +1862,9 @@
       <c r="E12" t="str">
         <v/>
       </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
       <c r="G12" t="str">
         <v/>
       </c>
@@ -1861,6 +1894,9 @@
       <c r="E13" t="str">
         <v/>
       </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
       <c r="G13" t="str">
         <v/>
       </c>
@@ -1890,6 +1926,9 @@
       <c r="E14" t="str">
         <v/>
       </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
       <c r="G14" t="str">
         <v/>
       </c>
@@ -1919,6 +1958,9 @@
       <c r="E15" t="str">
         <v/>
       </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
       <c r="G15" t="str">
         <v/>
       </c>
@@ -1948,6 +1990,9 @@
       <c r="E16" t="str">
         <v/>
       </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
       <c r="G16" t="str">
         <v/>
       </c>
@@ -1977,6 +2022,9 @@
       <c r="E17" t="str">
         <v/>
       </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
       <c r="G17" t="str">
         <v/>
       </c>
@@ -2006,6 +2054,9 @@
       <c r="E18" t="str">
         <v/>
       </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
       <c r="G18" t="str">
         <v/>
       </c>
@@ -2035,6 +2086,9 @@
       <c r="E19" t="str">
         <v/>
       </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
       <c r="G19" t="str">
         <v/>
       </c>
@@ -2064,6 +2118,9 @@
       <c r="E20" t="str">
         <v/>
       </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
       <c r="G20" t="str">
         <v/>
       </c>
@@ -2093,6 +2150,9 @@
       <c r="E21" t="str">
         <v/>
       </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
       <c r="G21" t="str">
         <v/>
       </c>
@@ -2122,6 +2182,9 @@
       <c r="E22" t="str">
         <v/>
       </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
       <c r="G22" t="str">
         <v/>
       </c>
@@ -2151,6 +2214,9 @@
       <c r="E23" t="str">
         <v/>
       </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
       <c r="G23" t="str">
         <v/>
       </c>
@@ -2180,6 +2246,9 @@
       <c r="E24" t="str">
         <v/>
       </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
       <c r="G24" t="str">
         <v/>
       </c>
@@ -2209,6 +2278,9 @@
       <c r="E25" t="str">
         <v/>
       </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
       <c r="G25" t="str">
         <v/>
       </c>
@@ -2238,6 +2310,9 @@
       <c r="E26" t="str">
         <v/>
       </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
       <c r="G26" t="str">
         <v/>
       </c>
@@ -2267,6 +2342,9 @@
       <c r="E27" t="str">
         <v/>
       </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
       <c r="G27" t="str">
         <v/>
       </c>
@@ -2296,6 +2374,9 @@
       <c r="E28" t="str">
         <v/>
       </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
       <c r="G28" t="str">
         <v/>
       </c>
@@ -2325,6 +2406,9 @@
       <c r="E29" t="str">
         <v/>
       </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
       <c r="G29" t="str">
         <v/>
       </c>
@@ -2354,6 +2438,9 @@
       <c r="E30" t="str">
         <v/>
       </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
       <c r="G30" t="str">
         <v/>
       </c>
@@ -2383,6 +2470,9 @@
       <c r="E31" t="str">
         <v/>
       </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
       <c r="G31" t="str">
         <v/>
       </c>
@@ -2412,6 +2502,9 @@
       <c r="E32" t="str">
         <v/>
       </c>
+      <c r="F32" t="str">
+        <v/>
+      </c>
       <c r="G32" t="str">
         <v/>
       </c>
@@ -2441,6 +2534,9 @@
       <c r="E33" t="str">
         <v/>
       </c>
+      <c r="F33" t="str">
+        <v/>
+      </c>
       <c r="G33" t="str">
         <v/>
       </c>
@@ -2470,6 +2566,9 @@
       <c r="E34" t="str">
         <v/>
       </c>
+      <c r="F34" t="str">
+        <v/>
+      </c>
       <c r="G34" t="str">
         <v/>
       </c>
@@ -2499,6 +2598,9 @@
       <c r="E35" t="str">
         <v/>
       </c>
+      <c r="F35" t="str">
+        <v/>
+      </c>
       <c r="G35" t="str">
         <v/>
       </c>
@@ -2528,6 +2630,9 @@
       <c r="E36" t="str">
         <v/>
       </c>
+      <c r="F36" t="str">
+        <v/>
+      </c>
       <c r="G36" t="str">
         <v/>
       </c>
@@ -2557,6 +2662,9 @@
       <c r="E37" t="str">
         <v/>
       </c>
+      <c r="F37" t="str">
+        <v/>
+      </c>
       <c r="G37" t="str">
         <v/>
       </c>
@@ -2586,6 +2694,9 @@
       <c r="E38" t="str">
         <v/>
       </c>
+      <c r="F38" t="str">
+        <v/>
+      </c>
       <c r="G38" t="str">
         <v/>
       </c>
@@ -2615,6 +2726,9 @@
       <c r="E39" t="str">
         <v/>
       </c>
+      <c r="F39" t="str">
+        <v/>
+      </c>
       <c r="G39" t="str">
         <v/>
       </c>
@@ -2644,6 +2758,9 @@
       <c r="E40" t="str">
         <v/>
       </c>
+      <c r="F40" t="str">
+        <v/>
+      </c>
       <c r="G40" t="str">
         <v/>
       </c>
@@ -2673,6 +2790,9 @@
       <c r="E41" t="str">
         <v/>
       </c>
+      <c r="F41" t="str">
+        <v/>
+      </c>
       <c r="G41" t="str">
         <v/>
       </c>
@@ -2702,6 +2822,9 @@
       <c r="E42" t="str">
         <v/>
       </c>
+      <c r="F42" t="str">
+        <v/>
+      </c>
       <c r="G42" t="str">
         <v/>
       </c>
@@ -2731,6 +2854,9 @@
       <c r="E43" t="str">
         <v/>
       </c>
+      <c r="F43" t="str">
+        <v/>
+      </c>
       <c r="G43" t="str">
         <v/>
       </c>
@@ -2760,6 +2886,9 @@
       <c r="E44" t="str">
         <v/>
       </c>
+      <c r="F44" t="str">
+        <v/>
+      </c>
       <c r="G44" t="str">
         <v/>
       </c>
@@ -2789,6 +2918,9 @@
       <c r="E45" t="str">
         <v/>
       </c>
+      <c r="F45" t="str">
+        <v/>
+      </c>
       <c r="G45" t="str">
         <v/>
       </c>
@@ -2818,6 +2950,9 @@
       <c r="E46" t="str">
         <v/>
       </c>
+      <c r="F46" t="str">
+        <v/>
+      </c>
       <c r="G46" t="str">
         <v/>
       </c>
@@ -2847,6 +2982,9 @@
       <c r="E47" t="str">
         <v/>
       </c>
+      <c r="F47" t="str">
+        <v/>
+      </c>
       <c r="G47" t="str">
         <v/>
       </c>
@@ -2876,6 +3014,9 @@
       <c r="E48" t="str">
         <v/>
       </c>
+      <c r="F48" t="str">
+        <v/>
+      </c>
       <c r="G48" t="str">
         <v/>
       </c>
@@ -2905,6 +3046,9 @@
       <c r="E49" t="str">
         <v/>
       </c>
+      <c r="F49" t="str">
+        <v/>
+      </c>
       <c r="G49" t="str">
         <v/>
       </c>
@@ -2934,6 +3078,9 @@
       <c r="E50" t="str">
         <v/>
       </c>
+      <c r="F50" t="str">
+        <v/>
+      </c>
       <c r="G50" t="str">
         <v/>
       </c>
@@ -2963,6 +3110,9 @@
       <c r="E51" t="str">
         <v/>
       </c>
+      <c r="F51" t="str">
+        <v/>
+      </c>
       <c r="G51" t="str">
         <v/>
       </c>
@@ -2992,6 +3142,9 @@
       <c r="E52" t="str">
         <v/>
       </c>
+      <c r="F52" t="str">
+        <v/>
+      </c>
       <c r="G52" t="str">
         <v/>
       </c>
@@ -3021,6 +3174,9 @@
       <c r="E53" t="str">
         <v/>
       </c>
+      <c r="F53" t="str">
+        <v/>
+      </c>
       <c r="G53" t="str">
         <v/>
       </c>
@@ -3050,6 +3206,9 @@
       <c r="E54" t="str">
         <v/>
       </c>
+      <c r="F54" t="str">
+        <v/>
+      </c>
       <c r="G54" t="str">
         <v/>
       </c>
@@ -3079,6 +3238,9 @@
       <c r="E55" t="str">
         <v/>
       </c>
+      <c r="F55" t="str">
+        <v/>
+      </c>
       <c r="G55" t="str">
         <v/>
       </c>
@@ -3108,6 +3270,9 @@
       <c r="E56" t="str">
         <v/>
       </c>
+      <c r="F56" t="str">
+        <v/>
+      </c>
       <c r="G56" t="str">
         <v/>
       </c>
@@ -3137,6 +3302,9 @@
       <c r="E57" t="str">
         <v/>
       </c>
+      <c r="F57" t="str">
+        <v/>
+      </c>
       <c r="G57" t="str">
         <v/>
       </c>
@@ -3166,6 +3334,9 @@
       <c r="E58" t="str">
         <v/>
       </c>
+      <c r="F58" t="str">
+        <v/>
+      </c>
       <c r="G58" t="str">
         <v/>
       </c>
@@ -3195,6 +3366,9 @@
       <c r="E59" t="str">
         <v/>
       </c>
+      <c r="F59" t="str">
+        <v/>
+      </c>
       <c r="G59" t="str">
         <v/>
       </c>
@@ -3224,6 +3398,9 @@
       <c r="E60" t="str">
         <v/>
       </c>
+      <c r="F60" t="str">
+        <v/>
+      </c>
       <c r="G60" t="str">
         <v/>
       </c>
@@ -3253,6 +3430,9 @@
       <c r="E61" t="str">
         <v/>
       </c>
+      <c r="F61" t="str">
+        <v/>
+      </c>
       <c r="G61" t="str">
         <v/>
       </c>
@@ -3282,6 +3462,9 @@
       <c r="E62" t="str">
         <v/>
       </c>
+      <c r="F62" t="str">
+        <v/>
+      </c>
       <c r="G62" t="str">
         <v/>
       </c>
@@ -3311,6 +3494,9 @@
       <c r="E63" t="str">
         <v/>
       </c>
+      <c r="F63" t="str">
+        <v/>
+      </c>
       <c r="G63" t="str">
         <v/>
       </c>
@@ -3340,6 +3526,9 @@
       <c r="E64" t="str">
         <v/>
       </c>
+      <c r="F64" t="str">
+        <v/>
+      </c>
       <c r="G64" t="str">
         <v/>
       </c>
@@ -3369,6 +3558,9 @@
       <c r="E65" t="str">
         <v/>
       </c>
+      <c r="F65" t="str">
+        <v/>
+      </c>
       <c r="G65" t="str">
         <v/>
       </c>
@@ -3398,6 +3590,9 @@
       <c r="E66" t="str">
         <v/>
       </c>
+      <c r="F66" t="str">
+        <v/>
+      </c>
       <c r="G66" t="str">
         <v/>
       </c>
@@ -3427,6 +3622,9 @@
       <c r="E67" t="str">
         <v/>
       </c>
+      <c r="F67" t="str">
+        <v/>
+      </c>
       <c r="G67" t="str">
         <v/>
       </c>
@@ -3456,6 +3654,9 @@
       <c r="E68" t="str">
         <v/>
       </c>
+      <c r="F68" t="str">
+        <v/>
+      </c>
       <c r="G68" t="str">
         <v/>
       </c>
@@ -3485,6 +3686,9 @@
       <c r="E69" t="str">
         <v/>
       </c>
+      <c r="F69" t="str">
+        <v/>
+      </c>
       <c r="G69" t="str">
         <v/>
       </c>
@@ -3514,6 +3718,9 @@
       <c r="E70" t="str">
         <v/>
       </c>
+      <c r="F70" t="str">
+        <v/>
+      </c>
       <c r="G70" t="str">
         <v/>
       </c>
@@ -3543,6 +3750,9 @@
       <c r="E71" t="str">
         <v/>
       </c>
+      <c r="F71" t="str">
+        <v/>
+      </c>
       <c r="G71" t="str">
         <v/>
       </c>
@@ -3572,6 +3782,9 @@
       <c r="E72" t="str">
         <v/>
       </c>
+      <c r="F72" t="str">
+        <v/>
+      </c>
       <c r="G72" t="str">
         <v/>
       </c>
@@ -3601,6 +3814,9 @@
       <c r="E73" t="str">
         <v/>
       </c>
+      <c r="F73" t="str">
+        <v/>
+      </c>
       <c r="G73" t="str">
         <v/>
       </c>
@@ -3630,6 +3846,9 @@
       <c r="E74" t="str">
         <v/>
       </c>
+      <c r="F74" t="str">
+        <v/>
+      </c>
       <c r="G74" t="str">
         <v/>
       </c>
@@ -3659,6 +3878,9 @@
       <c r="E75" t="str">
         <v/>
       </c>
+      <c r="F75" t="str">
+        <v/>
+      </c>
       <c r="G75" t="str">
         <v/>
       </c>
@@ -3688,6 +3910,9 @@
       <c r="E76" t="str">
         <v/>
       </c>
+      <c r="F76" t="str">
+        <v/>
+      </c>
       <c r="G76" t="str">
         <v/>
       </c>
@@ -3717,6 +3942,9 @@
       <c r="E77" t="str">
         <v/>
       </c>
+      <c r="F77" t="str">
+        <v/>
+      </c>
       <c r="G77" t="str">
         <v/>
       </c>
@@ -3746,6 +3974,9 @@
       <c r="E78" t="str">
         <v/>
       </c>
+      <c r="F78" t="str">
+        <v/>
+      </c>
       <c r="G78" t="str">
         <v/>
       </c>
@@ -3775,6 +4006,9 @@
       <c r="E79" t="str">
         <v/>
       </c>
+      <c r="F79" t="str">
+        <v/>
+      </c>
       <c r="G79" t="str">
         <v/>
       </c>
@@ -3804,6 +4038,9 @@
       <c r="E80" t="str">
         <v/>
       </c>
+      <c r="F80" t="str">
+        <v/>
+      </c>
       <c r="G80" t="str">
         <v/>
       </c>
@@ -3833,6 +4070,9 @@
       <c r="E81" t="str">
         <v/>
       </c>
+      <c r="F81" t="str">
+        <v/>
+      </c>
       <c r="G81" t="str">
         <v/>
       </c>
@@ -3862,6 +4102,9 @@
       <c r="E82" t="str">
         <v/>
       </c>
+      <c r="F82" t="str">
+        <v/>
+      </c>
       <c r="G82" t="str">
         <v/>
       </c>
@@ -3891,6 +4134,9 @@
       <c r="E83" t="str">
         <v/>
       </c>
+      <c r="F83" t="str">
+        <v/>
+      </c>
       <c r="G83" t="str">
         <v/>
       </c>
@@ -3920,6 +4166,9 @@
       <c r="E84" t="str">
         <v/>
       </c>
+      <c r="F84" t="str">
+        <v/>
+      </c>
       <c r="G84" t="str">
         <v/>
       </c>
@@ -3949,6 +4198,9 @@
       <c r="E85" t="str">
         <v/>
       </c>
+      <c r="F85" t="str">
+        <v/>
+      </c>
       <c r="G85" t="str">
         <v/>
       </c>
@@ -3978,6 +4230,9 @@
       <c r="E86" t="str">
         <v/>
       </c>
+      <c r="F86" t="str">
+        <v/>
+      </c>
       <c r="G86" t="str">
         <v/>
       </c>
@@ -4007,6 +4262,9 @@
       <c r="E87" t="str">
         <v/>
       </c>
+      <c r="F87" t="str">
+        <v/>
+      </c>
       <c r="G87" t="str">
         <v/>
       </c>
@@ -4036,6 +4294,9 @@
       <c r="E88" t="str">
         <v/>
       </c>
+      <c r="F88" t="str">
+        <v/>
+      </c>
       <c r="G88" t="str">
         <v/>
       </c>
@@ -4065,6 +4326,9 @@
       <c r="E89" t="str">
         <v/>
       </c>
+      <c r="F89" t="str">
+        <v/>
+      </c>
       <c r="G89" t="str">
         <v/>
       </c>
@@ -4094,6 +4358,9 @@
       <c r="E90" t="str">
         <v/>
       </c>
+      <c r="F90" t="str">
+        <v/>
+      </c>
       <c r="G90" t="str">
         <v/>
       </c>
@@ -4123,6 +4390,9 @@
       <c r="E91" t="str">
         <v/>
       </c>
+      <c r="F91" t="str">
+        <v/>
+      </c>
       <c r="G91" t="str">
         <v/>
       </c>
@@ -4152,6 +4422,9 @@
       <c r="E92" t="str">
         <v/>
       </c>
+      <c r="F92" t="str">
+        <v/>
+      </c>
       <c r="G92" t="str">
         <v/>
       </c>
@@ -4181,6 +4454,9 @@
       <c r="E93" t="str">
         <v/>
       </c>
+      <c r="F93" t="str">
+        <v/>
+      </c>
       <c r="G93" t="str">
         <v/>
       </c>
@@ -4210,6 +4486,9 @@
       <c r="E94" t="str">
         <v/>
       </c>
+      <c r="F94" t="str">
+        <v/>
+      </c>
       <c r="G94" t="str">
         <v/>
       </c>
@@ -4239,6 +4518,9 @@
       <c r="E95" t="str">
         <v/>
       </c>
+      <c r="F95" t="str">
+        <v/>
+      </c>
       <c r="G95" t="str">
         <v/>
       </c>
@@ -4268,6 +4550,9 @@
       <c r="E96" t="str">
         <v/>
       </c>
+      <c r="F96" t="str">
+        <v/>
+      </c>
       <c r="G96" t="str">
         <v/>
       </c>
@@ -4297,6 +4582,9 @@
       <c r="E97" t="str">
         <v/>
       </c>
+      <c r="F97" t="str">
+        <v/>
+      </c>
       <c r="G97" t="str">
         <v/>
       </c>
@@ -4326,6 +4614,9 @@
       <c r="E98" t="str">
         <v/>
       </c>
+      <c r="F98" t="str">
+        <v/>
+      </c>
       <c r="G98" t="str">
         <v/>
       </c>
@@ -4355,6 +4646,9 @@
       <c r="E99" t="str">
         <v/>
       </c>
+      <c r="F99" t="str">
+        <v/>
+      </c>
       <c r="G99" t="str">
         <v/>
       </c>
@@ -4384,6 +4678,9 @@
       <c r="E100" t="str">
         <v/>
       </c>
+      <c r="F100" t="str">
+        <v/>
+      </c>
       <c r="G100" t="str">
         <v/>
       </c>
@@ -4413,6 +4710,9 @@
       <c r="E101" t="str">
         <v/>
       </c>
+      <c r="F101" t="str">
+        <v/>
+      </c>
       <c r="G101" t="str">
         <v/>
       </c>
@@ -4442,6 +4742,9 @@
       <c r="E102" t="str">
         <v/>
       </c>
+      <c r="F102" t="str">
+        <v/>
+      </c>
       <c r="G102" t="str">
         <v/>
       </c>
@@ -4471,6 +4774,9 @@
       <c r="E103" t="str">
         <v/>
       </c>
+      <c r="F103" t="str">
+        <v/>
+      </c>
       <c r="G103" t="str">
         <v/>
       </c>
@@ -4500,6 +4806,9 @@
       <c r="E104" t="str">
         <v/>
       </c>
+      <c r="F104" t="str">
+        <v/>
+      </c>
       <c r="G104" t="str">
         <v/>
       </c>
@@ -4529,6 +4838,9 @@
       <c r="E105" t="str">
         <v/>
       </c>
+      <c r="F105" t="str">
+        <v/>
+      </c>
       <c r="G105" t="str">
         <v/>
       </c>
@@ -4558,6 +4870,9 @@
       <c r="E106" t="str">
         <v/>
       </c>
+      <c r="F106" t="str">
+        <v/>
+      </c>
       <c r="G106" t="str">
         <v/>
       </c>
@@ -4587,6 +4902,9 @@
       <c r="E107" t="str">
         <v/>
       </c>
+      <c r="F107" t="str">
+        <v/>
+      </c>
       <c r="G107" t="str">
         <v/>
       </c>
@@ -4616,6 +4934,9 @@
       <c r="E108" t="str">
         <v/>
       </c>
+      <c r="F108" t="str">
+        <v/>
+      </c>
       <c r="G108" t="str">
         <v/>
       </c>
@@ -4645,6 +4966,9 @@
       <c r="E109" t="str">
         <v/>
       </c>
+      <c r="F109" t="str">
+        <v/>
+      </c>
       <c r="G109" t="str">
         <v/>
       </c>
@@ -4674,6 +4998,9 @@
       <c r="E110" t="str">
         <v/>
       </c>
+      <c r="F110" t="str">
+        <v/>
+      </c>
       <c r="G110" t="str">
         <v/>
       </c>
@@ -4703,6 +5030,9 @@
       <c r="E111" t="str">
         <v/>
       </c>
+      <c r="F111" t="str">
+        <v/>
+      </c>
       <c r="G111" t="str">
         <v/>
       </c>
@@ -4732,6 +5062,9 @@
       <c r="E112" t="str">
         <v/>
       </c>
+      <c r="F112" t="str">
+        <v/>
+      </c>
       <c r="G112" t="str">
         <v/>
       </c>
@@ -4761,6 +5094,9 @@
       <c r="E113" t="str">
         <v/>
       </c>
+      <c r="F113" t="str">
+        <v/>
+      </c>
       <c r="G113" t="str">
         <v/>
       </c>
@@ -4790,6 +5126,9 @@
       <c r="E114" t="str">
         <v/>
       </c>
+      <c r="F114" t="str">
+        <v/>
+      </c>
       <c r="G114" t="str">
         <v/>
       </c>
@@ -4819,6 +5158,9 @@
       <c r="E115" t="str">
         <v/>
       </c>
+      <c r="F115" t="str">
+        <v/>
+      </c>
       <c r="G115" t="str">
         <v/>
       </c>
@@ -4848,6 +5190,9 @@
       <c r="E116" t="str">
         <v/>
       </c>
+      <c r="F116" t="str">
+        <v/>
+      </c>
       <c r="G116" t="str">
         <v/>
       </c>
@@ -4877,6 +5222,9 @@
       <c r="E117" t="str">
         <v/>
       </c>
+      <c r="F117" t="str">
+        <v/>
+      </c>
       <c r="G117" t="str">
         <v/>
       </c>
@@ -4906,6 +5254,9 @@
       <c r="E118" t="str">
         <v/>
       </c>
+      <c r="F118" t="str">
+        <v/>
+      </c>
       <c r="G118" t="str">
         <v/>
       </c>
@@ -4935,6 +5286,9 @@
       <c r="E119" t="str">
         <v/>
       </c>
+      <c r="F119" t="str">
+        <v/>
+      </c>
       <c r="G119" t="str">
         <v/>
       </c>
@@ -4964,6 +5318,9 @@
       <c r="E120" t="str">
         <v/>
       </c>
+      <c r="F120" t="str">
+        <v/>
+      </c>
       <c r="G120" t="str">
         <v/>
       </c>
@@ -4993,6 +5350,9 @@
       <c r="E121" t="str">
         <v/>
       </c>
+      <c r="F121" t="str">
+        <v/>
+      </c>
       <c r="G121" t="str">
         <v/>
       </c>
@@ -5022,6 +5382,9 @@
       <c r="E122" t="str">
         <v/>
       </c>
+      <c r="F122" t="str">
+        <v/>
+      </c>
       <c r="G122" t="str">
         <v/>
       </c>
@@ -5051,6 +5414,9 @@
       <c r="E123" t="str">
         <v/>
       </c>
+      <c r="F123" t="str">
+        <v/>
+      </c>
       <c r="G123" t="str">
         <v/>
       </c>
@@ -5080,6 +5446,9 @@
       <c r="E124" t="str">
         <v/>
       </c>
+      <c r="F124" t="str">
+        <v/>
+      </c>
       <c r="G124" t="str">
         <v/>
       </c>
@@ -5109,6 +5478,9 @@
       <c r="E125" t="str">
         <v/>
       </c>
+      <c r="F125" t="str">
+        <v/>
+      </c>
       <c r="G125" t="str">
         <v/>
       </c>
@@ -5138,6 +5510,9 @@
       <c r="E126" t="str">
         <v/>
       </c>
+      <c r="F126" t="str">
+        <v/>
+      </c>
       <c r="G126" t="str">
         <v/>
       </c>
@@ -5167,6 +5542,9 @@
       <c r="E127" t="str">
         <v/>
       </c>
+      <c r="F127" t="str">
+        <v/>
+      </c>
       <c r="G127" t="str">
         <v/>
       </c>
@@ -5196,6 +5574,9 @@
       <c r="E128" t="str">
         <v/>
       </c>
+      <c r="F128" t="str">
+        <v/>
+      </c>
       <c r="G128" t="str">
         <v/>
       </c>
@@ -5225,6 +5606,9 @@
       <c r="E129" t="str">
         <v/>
       </c>
+      <c r="F129" t="str">
+        <v/>
+      </c>
       <c r="G129" t="str">
         <v/>
       </c>
@@ -5254,6 +5638,9 @@
       <c r="E130" t="str">
         <v/>
       </c>
+      <c r="F130" t="str">
+        <v/>
+      </c>
       <c r="G130" t="str">
         <v/>
       </c>
@@ -5283,6 +5670,9 @@
       <c r="E131" t="str">
         <v/>
       </c>
+      <c r="F131" t="str">
+        <v/>
+      </c>
       <c r="G131" t="str">
         <v/>
       </c>
@@ -5312,6 +5702,9 @@
       <c r="E132" t="str">
         <v/>
       </c>
+      <c r="F132" t="str">
+        <v/>
+      </c>
       <c r="G132" t="str">
         <v/>
       </c>
@@ -5341,6 +5734,9 @@
       <c r="E133" t="str">
         <v/>
       </c>
+      <c r="F133" t="str">
+        <v/>
+      </c>
       <c r="G133" t="str">
         <v/>
       </c>
@@ -5370,6 +5766,9 @@
       <c r="E134" t="str">
         <v/>
       </c>
+      <c r="F134" t="str">
+        <v/>
+      </c>
       <c r="G134" t="str">
         <v/>
       </c>
@@ -5399,6 +5798,9 @@
       <c r="E135" t="str">
         <v/>
       </c>
+      <c r="F135" t="str">
+        <v/>
+      </c>
       <c r="G135" t="str">
         <v/>
       </c>
@@ -5428,6 +5830,9 @@
       <c r="E136" t="str">
         <v/>
       </c>
+      <c r="F136" t="str">
+        <v/>
+      </c>
       <c r="G136" t="str">
         <v/>
       </c>
@@ -5457,6 +5862,9 @@
       <c r="E137" t="str">
         <v/>
       </c>
+      <c r="F137" t="str">
+        <v/>
+      </c>
       <c r="G137" t="str">
         <v/>
       </c>
@@ -5486,6 +5894,9 @@
       <c r="E138" t="str">
         <v/>
       </c>
+      <c r="F138" t="str">
+        <v/>
+      </c>
       <c r="G138" t="str">
         <v/>
       </c>
@@ -5515,6 +5926,9 @@
       <c r="E139" t="str">
         <v/>
       </c>
+      <c r="F139" t="str">
+        <v/>
+      </c>
       <c r="G139" t="str">
         <v/>
       </c>
@@ -5544,6 +5958,9 @@
       <c r="E140" t="str">
         <v/>
       </c>
+      <c r="F140" t="str">
+        <v/>
+      </c>
       <c r="G140" t="str">
         <v/>
       </c>
@@ -5573,6 +5990,9 @@
       <c r="E141" t="str">
         <v/>
       </c>
+      <c r="F141" t="str">
+        <v/>
+      </c>
       <c r="G141" t="str">
         <v/>
       </c>
@@ -5602,6 +6022,9 @@
       <c r="E142" t="str">
         <v/>
       </c>
+      <c r="F142" t="str">
+        <v/>
+      </c>
       <c r="G142" t="str">
         <v/>
       </c>
@@ -5631,6 +6054,9 @@
       <c r="E143" t="str">
         <v/>
       </c>
+      <c r="F143" t="str">
+        <v/>
+      </c>
       <c r="G143" t="str">
         <v/>
       </c>
@@ -5660,6 +6086,9 @@
       <c r="E144" t="str">
         <v/>
       </c>
+      <c r="F144" t="str">
+        <v/>
+      </c>
       <c r="G144" t="str">
         <v/>
       </c>
@@ -5689,6 +6118,9 @@
       <c r="E145" t="str">
         <v/>
       </c>
+      <c r="F145" t="str">
+        <v/>
+      </c>
       <c r="G145" t="str">
         <v/>
       </c>
@@ -5718,6 +6150,9 @@
       <c r="E146" t="str">
         <v/>
       </c>
+      <c r="F146" t="str">
+        <v/>
+      </c>
       <c r="G146" t="str">
         <v/>
       </c>
@@ -5747,6 +6182,9 @@
       <c r="E147" t="str">
         <v/>
       </c>
+      <c r="F147" t="str">
+        <v/>
+      </c>
       <c r="G147" t="str">
         <v/>
       </c>
@@ -5776,6 +6214,9 @@
       <c r="E148" t="str">
         <v/>
       </c>
+      <c r="F148" t="str">
+        <v/>
+      </c>
       <c r="G148" t="str">
         <v/>
       </c>
@@ -5805,6 +6246,9 @@
       <c r="E149" t="str">
         <v/>
       </c>
+      <c r="F149" t="str">
+        <v/>
+      </c>
       <c r="G149" t="str">
         <v/>
       </c>
@@ -5834,6 +6278,9 @@
       <c r="E150" t="str">
         <v/>
       </c>
+      <c r="F150" t="str">
+        <v/>
+      </c>
       <c r="G150" t="str">
         <v/>
       </c>
@@ -5863,6 +6310,9 @@
       <c r="E151" t="str">
         <v/>
       </c>
+      <c r="F151" t="str">
+        <v/>
+      </c>
       <c r="G151" t="str">
         <v/>
       </c>
@@ -5892,6 +6342,9 @@
       <c r="E152" t="str">
         <v/>
       </c>
+      <c r="F152" t="str">
+        <v/>
+      </c>
       <c r="G152" t="str">
         <v/>
       </c>
@@ -5921,6 +6374,9 @@
       <c r="E153" t="str">
         <v/>
       </c>
+      <c r="F153" t="str">
+        <v/>
+      </c>
       <c r="G153" t="str">
         <v/>
       </c>
@@ -5950,6 +6406,9 @@
       <c r="E154" t="str">
         <v/>
       </c>
+      <c r="F154" t="str">
+        <v/>
+      </c>
       <c r="G154" t="str">
         <v/>
       </c>
@@ -5979,6 +6438,9 @@
       <c r="E155" t="str">
         <v/>
       </c>
+      <c r="F155" t="str">
+        <v/>
+      </c>
       <c r="G155" t="str">
         <v/>
       </c>
@@ -6008,6 +6470,9 @@
       <c r="E156" t="str">
         <v/>
       </c>
+      <c r="F156" t="str">
+        <v/>
+      </c>
       <c r="G156" t="str">
         <v/>
       </c>
@@ -6037,6 +6502,9 @@
       <c r="E157" t="str">
         <v/>
       </c>
+      <c r="F157" t="str">
+        <v/>
+      </c>
       <c r="G157" t="str">
         <v/>
       </c>
@@ -6066,6 +6534,9 @@
       <c r="E158" t="str">
         <v/>
       </c>
+      <c r="F158" t="str">
+        <v/>
+      </c>
       <c r="G158" t="str">
         <v/>
       </c>
@@ -6095,6 +6566,9 @@
       <c r="E159" t="str">
         <v/>
       </c>
+      <c r="F159" t="str">
+        <v/>
+      </c>
       <c r="G159" t="str">
         <v/>
       </c>
@@ -6124,6 +6598,9 @@
       <c r="E160" t="str">
         <v/>
       </c>
+      <c r="F160" t="str">
+        <v/>
+      </c>
       <c r="G160" t="str">
         <v/>
       </c>
@@ -6153,6 +6630,9 @@
       <c r="E161" t="str">
         <v/>
       </c>
+      <c r="F161" t="str">
+        <v/>
+      </c>
       <c r="G161" t="str">
         <v/>
       </c>
@@ -6182,6 +6662,9 @@
       <c r="E162" t="str">
         <v/>
       </c>
+      <c r="F162" t="str">
+        <v/>
+      </c>
       <c r="G162" t="str">
         <v/>
       </c>
@@ -6211,6 +6694,9 @@
       <c r="E163" t="str">
         <v/>
       </c>
+      <c r="F163" t="str">
+        <v/>
+      </c>
       <c r="G163" t="str">
         <v/>
       </c>
@@ -6240,6 +6726,9 @@
       <c r="E164" t="str">
         <v/>
       </c>
+      <c r="F164" t="str">
+        <v/>
+      </c>
       <c r="G164" t="str">
         <v/>
       </c>
@@ -6269,6 +6758,9 @@
       <c r="E165" t="str">
         <v/>
       </c>
+      <c r="F165" t="str">
+        <v/>
+      </c>
       <c r="G165" t="str">
         <v/>
       </c>
@@ -6298,6 +6790,9 @@
       <c r="E166" t="str">
         <v/>
       </c>
+      <c r="F166" t="str">
+        <v/>
+      </c>
       <c r="G166" t="str">
         <v/>
       </c>
@@ -6327,6 +6822,9 @@
       <c r="E167" t="str">
         <v/>
       </c>
+      <c r="F167" t="str">
+        <v/>
+      </c>
       <c r="G167" t="str">
         <v/>
       </c>
@@ -6356,6 +6854,9 @@
       <c r="E168" t="str">
         <v/>
       </c>
+      <c r="F168" t="str">
+        <v/>
+      </c>
       <c r="G168" t="str">
         <v/>
       </c>
@@ -6385,6 +6886,9 @@
       <c r="E169" t="str">
         <v/>
       </c>
+      <c r="F169" t="str">
+        <v/>
+      </c>
       <c r="G169" t="str">
         <v/>
       </c>
@@ -6414,6 +6918,9 @@
       <c r="E170" t="str">
         <v/>
       </c>
+      <c r="F170" t="str">
+        <v/>
+      </c>
       <c r="G170" t="str">
         <v/>
       </c>
@@ -6443,6 +6950,9 @@
       <c r="E171" t="str">
         <v/>
       </c>
+      <c r="F171" t="str">
+        <v/>
+      </c>
       <c r="G171" t="str">
         <v/>
       </c>
@@ -6472,6 +6982,9 @@
       <c r="E172" t="str">
         <v/>
       </c>
+      <c r="F172" t="str">
+        <v/>
+      </c>
       <c r="G172" t="str">
         <v/>
       </c>
@@ -6501,6 +7014,9 @@
       <c r="E173" t="str">
         <v/>
       </c>
+      <c r="F173" t="str">
+        <v/>
+      </c>
       <c r="G173" t="str">
         <v/>
       </c>
@@ -6530,6 +7046,9 @@
       <c r="E174" t="str">
         <v/>
       </c>
+      <c r="F174" t="str">
+        <v/>
+      </c>
       <c r="G174" t="str">
         <v/>
       </c>
@@ -6559,6 +7078,9 @@
       <c r="E175" t="str">
         <v/>
       </c>
+      <c r="F175" t="str">
+        <v/>
+      </c>
       <c r="G175" t="str">
         <v/>
       </c>
@@ -6588,6 +7110,9 @@
       <c r="E176" t="str">
         <v/>
       </c>
+      <c r="F176" t="str">
+        <v/>
+      </c>
       <c r="G176" t="str">
         <v/>
       </c>
@@ -6617,6 +7142,9 @@
       <c r="E177" t="str">
         <v/>
       </c>
+      <c r="F177" t="str">
+        <v/>
+      </c>
       <c r="G177" t="str">
         <v/>
       </c>
@@ -6646,6 +7174,9 @@
       <c r="E178" t="str">
         <v/>
       </c>
+      <c r="F178" t="str">
+        <v/>
+      </c>
       <c r="G178" t="str">
         <v/>
       </c>
@@ -6675,6 +7206,9 @@
       <c r="E179" t="str">
         <v/>
       </c>
+      <c r="F179" t="str">
+        <v/>
+      </c>
       <c r="G179" t="str">
         <v/>
       </c>
@@ -6704,6 +7238,9 @@
       <c r="E180" t="str">
         <v/>
       </c>
+      <c r="F180" t="str">
+        <v/>
+      </c>
       <c r="G180" t="str">
         <v/>
       </c>
@@ -6733,6 +7270,9 @@
       <c r="E181" t="str">
         <v/>
       </c>
+      <c r="F181" t="str">
+        <v/>
+      </c>
       <c r="G181" t="str">
         <v/>
       </c>
@@ -6762,6 +7302,9 @@
       <c r="E182" t="str">
         <v/>
       </c>
+      <c r="F182" t="str">
+        <v/>
+      </c>
       <c r="G182" t="str">
         <v/>
       </c>
@@ -6791,6 +7334,9 @@
       <c r="E183" t="str">
         <v/>
       </c>
+      <c r="F183" t="str">
+        <v/>
+      </c>
       <c r="G183" t="str">
         <v/>
       </c>
@@ -6820,6 +7366,9 @@
       <c r="E184" t="str">
         <v/>
       </c>
+      <c r="F184" t="str">
+        <v/>
+      </c>
       <c r="G184" t="str">
         <v/>
       </c>
@@ -6849,6 +7398,9 @@
       <c r="E185" t="str">
         <v/>
       </c>
+      <c r="F185" t="str">
+        <v/>
+      </c>
       <c r="G185" t="str">
         <v/>
       </c>
@@ -6878,6 +7430,9 @@
       <c r="E186" t="str">
         <v/>
       </c>
+      <c r="F186" t="str">
+        <v/>
+      </c>
       <c r="G186" t="str">
         <v/>
       </c>
@@ -6907,6 +7462,9 @@
       <c r="E187" t="str">
         <v/>
       </c>
+      <c r="F187" t="str">
+        <v/>
+      </c>
       <c r="G187" t="str">
         <v/>
       </c>
@@ -6936,6 +7494,9 @@
       <c r="E188" t="str">
         <v/>
       </c>
+      <c r="F188" t="str">
+        <v/>
+      </c>
       <c r="G188" t="str">
         <v/>
       </c>
@@ -6965,6 +7526,9 @@
       <c r="E189" t="str">
         <v/>
       </c>
+      <c r="F189" t="str">
+        <v/>
+      </c>
       <c r="G189" t="str">
         <v/>
       </c>
@@ -6994,6 +7558,9 @@
       <c r="E190" t="str">
         <v/>
       </c>
+      <c r="F190" t="str">
+        <v/>
+      </c>
       <c r="G190" t="str">
         <v/>
       </c>
@@ -7023,6 +7590,9 @@
       <c r="E191" t="str">
         <v/>
       </c>
+      <c r="F191" t="str">
+        <v/>
+      </c>
       <c r="G191" t="str">
         <v/>
       </c>
@@ -7052,6 +7622,9 @@
       <c r="E192" t="str">
         <v/>
       </c>
+      <c r="F192" t="str">
+        <v/>
+      </c>
       <c r="G192" t="str">
         <v/>
       </c>
@@ -7081,6 +7654,9 @@
       <c r="E193" t="str">
         <v/>
       </c>
+      <c r="F193" t="str">
+        <v/>
+      </c>
       <c r="G193" t="str">
         <v/>
       </c>
@@ -7110,6 +7686,9 @@
       <c r="E194" t="str">
         <v/>
       </c>
+      <c r="F194" t="str">
+        <v/>
+      </c>
       <c r="G194" t="str">
         <v/>
       </c>
@@ -7139,6 +7718,9 @@
       <c r="E195" t="str">
         <v/>
       </c>
+      <c r="F195" t="str">
+        <v/>
+      </c>
       <c r="G195" t="str">
         <v/>
       </c>
@@ -7168,6 +7750,9 @@
       <c r="E196" t="str">
         <v/>
       </c>
+      <c r="F196" t="str">
+        <v/>
+      </c>
       <c r="G196" t="str">
         <v/>
       </c>
@@ -7197,6 +7782,9 @@
       <c r="E197" t="str">
         <v/>
       </c>
+      <c r="F197" t="str">
+        <v/>
+      </c>
       <c r="G197" t="str">
         <v/>
       </c>
@@ -7226,6 +7814,9 @@
       <c r="E198" t="str">
         <v/>
       </c>
+      <c r="F198" t="str">
+        <v/>
+      </c>
       <c r="G198" t="str">
         <v/>
       </c>
@@ -7255,6 +7846,9 @@
       <c r="E199" t="str">
         <v/>
       </c>
+      <c r="F199" t="str">
+        <v/>
+      </c>
       <c r="G199" t="str">
         <v/>
       </c>
@@ -7284,6 +7878,9 @@
       <c r="E200" t="str">
         <v/>
       </c>
+      <c r="F200" t="str">
+        <v/>
+      </c>
       <c r="G200" t="str">
         <v/>
       </c>
@@ -7313,6 +7910,9 @@
       <c r="E201" t="str">
         <v/>
       </c>
+      <c r="F201" t="str">
+        <v/>
+      </c>
       <c r="G201" t="str">
         <v/>
       </c>
@@ -7342,6 +7942,9 @@
       <c r="E202" t="str">
         <v/>
       </c>
+      <c r="F202" t="str">
+        <v/>
+      </c>
       <c r="G202" t="str">
         <v/>
       </c>
@@ -7371,6 +7974,9 @@
       <c r="E203" t="str">
         <v/>
       </c>
+      <c r="F203" t="str">
+        <v/>
+      </c>
       <c r="G203" t="str">
         <v/>
       </c>
@@ -7400,6 +8006,9 @@
       <c r="E204" t="str">
         <v/>
       </c>
+      <c r="F204" t="str">
+        <v/>
+      </c>
       <c r="G204" t="str">
         <v/>
       </c>
@@ -7429,6 +8038,9 @@
       <c r="E205" t="str">
         <v/>
       </c>
+      <c r="F205" t="str">
+        <v/>
+      </c>
       <c r="G205" t="str">
         <v/>
       </c>
@@ -7458,6 +8070,9 @@
       <c r="E206" t="str">
         <v/>
       </c>
+      <c r="F206" t="str">
+        <v/>
+      </c>
       <c r="G206" t="str">
         <v/>
       </c>
@@ -7487,6 +8102,9 @@
       <c r="E207" t="str">
         <v/>
       </c>
+      <c r="F207" t="str">
+        <v/>
+      </c>
       <c r="G207" t="str">
         <v/>
       </c>
@@ -7516,6 +8134,9 @@
       <c r="E208" t="str">
         <v/>
       </c>
+      <c r="F208" t="str">
+        <v/>
+      </c>
       <c r="G208" t="str">
         <v/>
       </c>
@@ -7545,6 +8166,9 @@
       <c r="E209" t="str">
         <v/>
       </c>
+      <c r="F209" t="str">
+        <v/>
+      </c>
       <c r="G209" t="str">
         <v/>
       </c>
@@ -7574,6 +8198,9 @@
       <c r="E210" t="str">
         <v/>
       </c>
+      <c r="F210" t="str">
+        <v/>
+      </c>
       <c r="G210" t="str">
         <v/>
       </c>
@@ -7603,6 +8230,9 @@
       <c r="E211" t="str">
         <v/>
       </c>
+      <c r="F211" t="str">
+        <v/>
+      </c>
       <c r="G211" t="str">
         <v/>
       </c>
@@ -7632,6 +8262,9 @@
       <c r="E212" t="str">
         <v/>
       </c>
+      <c r="F212" t="str">
+        <v/>
+      </c>
       <c r="G212" t="str">
         <v/>
       </c>
@@ -7661,6 +8294,9 @@
       <c r="E213" t="str">
         <v/>
       </c>
+      <c r="F213" t="str">
+        <v/>
+      </c>
       <c r="G213" t="str">
         <v/>
       </c>
@@ -7690,6 +8326,9 @@
       <c r="E214" t="str">
         <v/>
       </c>
+      <c r="F214" t="str">
+        <v/>
+      </c>
       <c r="G214" t="str">
         <v/>
       </c>
@@ -7719,6 +8358,9 @@
       <c r="E215" t="str">
         <v/>
       </c>
+      <c r="F215" t="str">
+        <v/>
+      </c>
       <c r="G215" t="str">
         <v/>
       </c>
@@ -7748,6 +8390,9 @@
       <c r="E216" t="str">
         <v/>
       </c>
+      <c r="F216" t="str">
+        <v/>
+      </c>
       <c r="G216" t="str">
         <v/>
       </c>
@@ -7777,6 +8422,9 @@
       <c r="E217" t="str">
         <v/>
       </c>
+      <c r="F217" t="str">
+        <v/>
+      </c>
       <c r="G217" t="str">
         <v/>
       </c>
@@ -7806,6 +8454,9 @@
       <c r="E218" t="str">
         <v/>
       </c>
+      <c r="F218" t="str">
+        <v/>
+      </c>
       <c r="G218" t="str">
         <v/>
       </c>
@@ -7835,6 +8486,9 @@
       <c r="E219" t="str">
         <v/>
       </c>
+      <c r="F219" t="str">
+        <v/>
+      </c>
       <c r="G219" t="str">
         <v/>
       </c>
@@ -7864,6 +8518,9 @@
       <c r="E220" t="str">
         <v/>
       </c>
+      <c r="F220" t="str">
+        <v/>
+      </c>
       <c r="G220" t="str">
         <v/>
       </c>
@@ -7893,6 +8550,9 @@
       <c r="E221" t="str">
         <v/>
       </c>
+      <c r="F221" t="str">
+        <v/>
+      </c>
       <c r="G221" t="str">
         <v/>
       </c>
@@ -7922,6 +8582,9 @@
       <c r="E222" t="str">
         <v/>
       </c>
+      <c r="F222" t="str">
+        <v/>
+      </c>
       <c r="G222" t="str">
         <v/>
       </c>
@@ -7951,6 +8614,9 @@
       <c r="E223" t="str">
         <v/>
       </c>
+      <c r="F223" t="str">
+        <v/>
+      </c>
       <c r="G223" t="str">
         <v/>
       </c>
@@ -7980,6 +8646,9 @@
       <c r="E224" t="str">
         <v/>
       </c>
+      <c r="F224" t="str">
+        <v/>
+      </c>
       <c r="G224" t="str">
         <v/>
       </c>
@@ -8009,6 +8678,9 @@
       <c r="E225" t="str">
         <v/>
       </c>
+      <c r="F225" t="str">
+        <v/>
+      </c>
       <c r="G225" t="str">
         <v/>
       </c>
@@ -8038,6 +8710,9 @@
       <c r="E226" t="str">
         <v/>
       </c>
+      <c r="F226" t="str">
+        <v/>
+      </c>
       <c r="G226" t="str">
         <v/>
       </c>
@@ -8067,6 +8742,9 @@
       <c r="E227" t="str">
         <v/>
       </c>
+      <c r="F227" t="str">
+        <v/>
+      </c>
       <c r="G227" t="str">
         <v/>
       </c>
@@ -8096,6 +8774,9 @@
       <c r="E228" t="str">
         <v/>
       </c>
+      <c r="F228" t="str">
+        <v/>
+      </c>
       <c r="G228" t="str">
         <v/>
       </c>
@@ -8125,6 +8806,9 @@
       <c r="E229" t="str">
         <v/>
       </c>
+      <c r="F229" t="str">
+        <v/>
+      </c>
       <c r="G229" t="str">
         <v/>
       </c>
@@ -8154,6 +8838,9 @@
       <c r="E230" t="str">
         <v/>
       </c>
+      <c r="F230" t="str">
+        <v/>
+      </c>
       <c r="G230" t="str">
         <v/>
       </c>
@@ -8183,6 +8870,9 @@
       <c r="E231" t="str">
         <v/>
       </c>
+      <c r="F231" t="str">
+        <v/>
+      </c>
       <c r="G231" t="str">
         <v/>
       </c>
@@ -8212,6 +8902,9 @@
       <c r="E232" t="str">
         <v/>
       </c>
+      <c r="F232" t="str">
+        <v/>
+      </c>
       <c r="G232" t="str">
         <v/>
       </c>
@@ -8241,6 +8934,9 @@
       <c r="E233" t="str">
         <v/>
       </c>
+      <c r="F233" t="str">
+        <v/>
+      </c>
       <c r="G233" t="str">
         <v/>
       </c>
@@ -8270,6 +8966,9 @@
       <c r="E234" t="str">
         <v/>
       </c>
+      <c r="F234" t="str">
+        <v/>
+      </c>
       <c r="G234" t="str">
         <v/>
       </c>
@@ -8299,6 +8998,9 @@
       <c r="E235" t="str">
         <v/>
       </c>
+      <c r="F235" t="str">
+        <v/>
+      </c>
       <c r="G235" t="str">
         <v/>
       </c>
@@ -8328,6 +9030,9 @@
       <c r="E236" t="str">
         <v/>
       </c>
+      <c r="F236" t="str">
+        <v/>
+      </c>
       <c r="G236" t="str">
         <v/>
       </c>
@@ -8357,6 +9062,9 @@
       <c r="E237" t="str">
         <v/>
       </c>
+      <c r="F237" t="str">
+        <v/>
+      </c>
       <c r="G237" t="str">
         <v/>
       </c>
@@ -8386,6 +9094,9 @@
       <c r="E238" t="str">
         <v/>
       </c>
+      <c r="F238" t="str">
+        <v/>
+      </c>
       <c r="G238" t="str">
         <v/>
       </c>
@@ -8415,6 +9126,9 @@
       <c r="E239" t="str">
         <v/>
       </c>
+      <c r="F239" t="str">
+        <v/>
+      </c>
       <c r="G239" t="str">
         <v/>
       </c>
@@ -8444,6 +9158,9 @@
       <c r="E240" t="str">
         <v/>
       </c>
+      <c r="F240" t="str">
+        <v/>
+      </c>
       <c r="G240" t="str">
         <v/>
       </c>
@@ -8473,6 +9190,9 @@
       <c r="E241" t="str">
         <v/>
       </c>
+      <c r="F241" t="str">
+        <v/>
+      </c>
       <c r="G241" t="str">
         <v/>
       </c>
@@ -8502,6 +9222,9 @@
       <c r="E242" t="str">
         <v/>
       </c>
+      <c r="F242" t="str">
+        <v/>
+      </c>
       <c r="G242" t="str">
         <v/>
       </c>
@@ -8531,6 +9254,9 @@
       <c r="E243" t="str">
         <v/>
       </c>
+      <c r="F243" t="str">
+        <v/>
+      </c>
       <c r="G243" t="str">
         <v/>
       </c>
@@ -8560,6 +9286,9 @@
       <c r="E244" t="str">
         <v/>
       </c>
+      <c r="F244" t="str">
+        <v/>
+      </c>
       <c r="G244" t="str">
         <v/>
       </c>
@@ -8589,6 +9318,9 @@
       <c r="E245" t="str">
         <v/>
       </c>
+      <c r="F245" t="str">
+        <v/>
+      </c>
       <c r="G245" t="str">
         <v/>
       </c>
@@ -8618,6 +9350,9 @@
       <c r="E246" t="str">
         <v/>
       </c>
+      <c r="F246" t="str">
+        <v/>
+      </c>
       <c r="G246" t="str">
         <v/>
       </c>
@@ -8647,6 +9382,9 @@
       <c r="E247" t="str">
         <v/>
       </c>
+      <c r="F247" t="str">
+        <v/>
+      </c>
       <c r="G247" t="str">
         <v/>
       </c>
@@ -8676,6 +9414,9 @@
       <c r="E248" t="str">
         <v/>
       </c>
+      <c r="F248" t="str">
+        <v/>
+      </c>
       <c r="G248" t="str">
         <v/>
       </c>
@@ -8705,6 +9446,9 @@
       <c r="E249" t="str">
         <v/>
       </c>
+      <c r="F249" t="str">
+        <v/>
+      </c>
       <c r="G249" t="str">
         <v/>
       </c>
@@ -8734,6 +9478,9 @@
       <c r="E250" t="str">
         <v/>
       </c>
+      <c r="F250" t="str">
+        <v/>
+      </c>
       <c r="G250" t="str">
         <v/>
       </c>
@@ -8763,6 +9510,9 @@
       <c r="E251" t="str">
         <v/>
       </c>
+      <c r="F251" t="str">
+        <v/>
+      </c>
       <c r="G251" t="str">
         <v/>
       </c>
@@ -8792,6 +9542,9 @@
       <c r="E252" t="str">
         <v/>
       </c>
+      <c r="F252" t="str">
+        <v/>
+      </c>
       <c r="G252" t="str">
         <v/>
       </c>
@@ -8821,6 +9574,9 @@
       <c r="E253" t="str">
         <v/>
       </c>
+      <c r="F253" t="str">
+        <v/>
+      </c>
       <c r="G253" t="str">
         <v/>
       </c>
@@ -8850,6 +9606,9 @@
       <c r="E254" t="str">
         <v/>
       </c>
+      <c r="F254" t="str">
+        <v/>
+      </c>
       <c r="G254" t="str">
         <v/>
       </c>
@@ -8879,6 +9638,9 @@
       <c r="E255" t="str">
         <v/>
       </c>
+      <c r="F255" t="str">
+        <v/>
+      </c>
       <c r="G255" t="str">
         <v/>
       </c>
@@ -8908,6 +9670,9 @@
       <c r="E256" t="str">
         <v/>
       </c>
+      <c r="F256" t="str">
+        <v/>
+      </c>
       <c r="G256" t="str">
         <v/>
       </c>
@@ -8936,6 +9701,9 @@
       </c>
       <c r="E257" t="str">
         <v>Hand Cash</v>
+      </c>
+      <c r="F257" t="str">
+        <v/>
       </c>
       <c r="G257" t="str">
         <v/>

</xml_diff>

<commit_message>
added google sheet & drive backup
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -464,6 +464,9 @@
       <c r="E2" t="str">
         <v>Hand Cash</v>
       </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
       <c r="G2" t="str">
         <v/>
       </c>
@@ -474,6 +477,9 @@
         <v/>
       </c>
       <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
         <v/>
       </c>
     </row>
@@ -493,6 +499,9 @@
       <c r="E3" t="str">
         <v>Dutch Bangla Bank</v>
       </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
       <c r="G3" t="str">
         <v/>
       </c>
@@ -525,6 +534,9 @@
       <c r="E4" t="str">
         <v/>
       </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
       <c r="G4" t="str">
         <v/>
       </c>
@@ -557,6 +569,9 @@
       <c r="E5" t="str">
         <v/>
       </c>
+      <c r="F5" t="str">
+        <v/>
+      </c>
       <c r="G5" t="str">
         <v/>
       </c>
@@ -589,6 +604,9 @@
       <c r="E6" t="str">
         <v/>
       </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
       <c r="G6" t="str">
         <v/>
       </c>
@@ -621,6 +639,9 @@
       <c r="E7" t="str">
         <v/>
       </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
       <c r="G7" t="str">
         <v/>
       </c>
@@ -653,6 +674,9 @@
       <c r="E8" t="str">
         <v/>
       </c>
+      <c r="F8" t="str">
+        <v/>
+      </c>
       <c r="G8" t="str">
         <v/>
       </c>
@@ -685,6 +709,9 @@
       <c r="E9" t="str">
         <v/>
       </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
       <c r="G9" t="str">
         <v/>
       </c>
@@ -717,6 +744,9 @@
       <c r="E10" t="str">
         <v/>
       </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
       <c r="G10" t="str">
         <v/>
       </c>
@@ -749,6 +779,9 @@
       <c r="E11" t="str">
         <v/>
       </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
       <c r="G11" t="str">
         <v/>
       </c>
@@ -781,6 +814,9 @@
       <c r="E12" t="str">
         <v/>
       </c>
+      <c r="F12" t="str">
+        <v/>
+      </c>
       <c r="G12" t="str">
         <v/>
       </c>
@@ -813,6 +849,9 @@
       <c r="E13" t="str">
         <v/>
       </c>
+      <c r="F13" t="str">
+        <v/>
+      </c>
       <c r="G13" t="str">
         <v/>
       </c>
@@ -845,6 +884,9 @@
       <c r="E14" t="str">
         <v/>
       </c>
+      <c r="F14" t="str">
+        <v/>
+      </c>
       <c r="G14" t="str">
         <v/>
       </c>
@@ -877,6 +919,9 @@
       <c r="E15" t="str">
         <v/>
       </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
       <c r="G15" t="str">
         <v/>
       </c>
@@ -909,6 +954,9 @@
       <c r="E16" t="str">
         <v/>
       </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
       <c r="G16" t="str">
         <v/>
       </c>
@@ -941,6 +989,9 @@
       <c r="E17" t="str">
         <v/>
       </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
       <c r="G17" t="str">
         <v/>
       </c>
@@ -973,6 +1024,9 @@
       <c r="E18" t="str">
         <v/>
       </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
       <c r="G18" t="str">
         <v/>
       </c>
@@ -1005,6 +1059,9 @@
       <c r="E19" t="str">
         <v/>
       </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
       <c r="G19" t="str">
         <v/>
       </c>
@@ -1037,6 +1094,9 @@
       <c r="E20" t="str">
         <v/>
       </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
       <c r="G20" t="str">
         <v/>
       </c>
@@ -1069,6 +1129,9 @@
       <c r="E21" t="str">
         <v/>
       </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
       <c r="G21" t="str">
         <v/>
       </c>
@@ -1101,6 +1164,9 @@
       <c r="E22" t="str">
         <v/>
       </c>
+      <c r="F22" t="str">
+        <v/>
+      </c>
       <c r="G22" t="str">
         <v/>
       </c>
@@ -1133,6 +1199,9 @@
       <c r="E23" t="str">
         <v/>
       </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
       <c r="G23" t="str">
         <v/>
       </c>
@@ -1165,6 +1234,9 @@
       <c r="E24" t="str">
         <v/>
       </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
       <c r="G24" t="str">
         <v/>
       </c>
@@ -1197,6 +1269,9 @@
       <c r="E25" t="str">
         <v/>
       </c>
+      <c r="F25" t="str">
+        <v/>
+      </c>
       <c r="G25" t="str">
         <v/>
       </c>
@@ -1229,6 +1304,9 @@
       <c r="E26" t="str">
         <v/>
       </c>
+      <c r="F26" t="str">
+        <v/>
+      </c>
       <c r="G26" t="str">
         <v/>
       </c>
@@ -1261,6 +1339,9 @@
       <c r="E27" t="str">
         <v/>
       </c>
+      <c r="F27" t="str">
+        <v/>
+      </c>
       <c r="G27" t="str">
         <v/>
       </c>
@@ -1293,6 +1374,9 @@
       <c r="E28" t="str">
         <v/>
       </c>
+      <c r="F28" t="str">
+        <v/>
+      </c>
       <c r="G28" t="str">
         <v/>
       </c>
@@ -1325,6 +1409,9 @@
       <c r="E29" t="str">
         <v/>
       </c>
+      <c r="F29" t="str">
+        <v/>
+      </c>
       <c r="G29" t="str">
         <v/>
       </c>
@@ -1357,6 +1444,9 @@
       <c r="E30" t="str">
         <v/>
       </c>
+      <c r="F30" t="str">
+        <v/>
+      </c>
       <c r="G30" t="str">
         <v/>
       </c>
@@ -1389,6 +1479,9 @@
       <c r="E31" t="str">
         <v/>
       </c>
+      <c r="F31" t="str">
+        <v/>
+      </c>
       <c r="G31" t="str">
         <v/>
       </c>
@@ -1419,6 +1512,9 @@
         <v>2025-12-01</v>
       </c>
       <c r="E32" t="str">
+        <v/>
+      </c>
+      <c r="F32" t="str">
         <v/>
       </c>
       <c r="G32" t="str">
@@ -1459,7 +1555,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1471,6 +1567,15 @@
       <c r="B1" t="str">
         <v>relation</v>
       </c>
+      <c r="C1" t="str">
+        <v>email</v>
+      </c>
+      <c r="D1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="E1" t="str">
+        <v>notes</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1479,10 +1584,19 @@
       <c r="B2" t="str">
         <v>Sister</v>
       </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated index.html to filter and display only active family members in various sections, enhancing the user experience. Added contributor badges for expenses and improved the display of family member details. Updated finance_data.xlsx for compatibility with these changes.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -1597,7 +1597,7 @@
         <v/>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1674,6 +1674,9 @@
       <c r="G2" t="str">
         <v>equal</v>
       </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
       <c r="I2" t="str">
         <v/>
       </c>
@@ -1706,6 +1709,12 @@
       <c r="F3" t="str">
         <v/>
       </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="str">
+        <v/>
+      </c>
       <c r="I3" t="str">
         <v/>
       </c>
@@ -1738,6 +1747,12 @@
       <c r="F4" t="str">
         <v/>
       </c>
+      <c r="G4" t="str">
+        <v/>
+      </c>
+      <c r="H4" t="str">
+        <v/>
+      </c>
       <c r="I4" t="str">
         <v/>
       </c>
@@ -1770,6 +1785,12 @@
       <c r="F5" t="str">
         <v/>
       </c>
+      <c r="G5" t="str">
+        <v/>
+      </c>
+      <c r="H5" t="str">
+        <v/>
+      </c>
       <c r="I5" t="str">
         <v/>
       </c>
@@ -1802,6 +1823,12 @@
       <c r="F6" t="str">
         <v/>
       </c>
+      <c r="G6" t="str">
+        <v/>
+      </c>
+      <c r="H6" t="str">
+        <v/>
+      </c>
       <c r="I6" t="str">
         <v/>
       </c>
@@ -1834,6 +1861,12 @@
       <c r="F7" t="str">
         <v/>
       </c>
+      <c r="G7" t="str">
+        <v/>
+      </c>
+      <c r="H7" t="str">
+        <v/>
+      </c>
       <c r="I7" t="str">
         <v/>
       </c>
@@ -1866,6 +1899,12 @@
       <c r="F8" t="str">
         <v/>
       </c>
+      <c r="G8" t="str">
+        <v/>
+      </c>
+      <c r="H8" t="str">
+        <v/>
+      </c>
       <c r="I8" t="str">
         <v/>
       </c>
@@ -1898,6 +1937,12 @@
       <c r="F9" t="str">
         <v/>
       </c>
+      <c r="G9" t="str">
+        <v/>
+      </c>
+      <c r="H9" t="str">
+        <v/>
+      </c>
       <c r="I9" t="str">
         <v/>
       </c>
@@ -1930,6 +1975,12 @@
       <c r="F10" t="str">
         <v/>
       </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+      <c r="H10" t="str">
+        <v/>
+      </c>
       <c r="I10" t="str">
         <v/>
       </c>
@@ -1962,6 +2013,12 @@
       <c r="F11" t="str">
         <v/>
       </c>
+      <c r="G11" t="str">
+        <v/>
+      </c>
+      <c r="H11" t="str">
+        <v/>
+      </c>
       <c r="I11" t="str">
         <v/>
       </c>
@@ -1994,6 +2051,12 @@
       <c r="F12" t="str">
         <v/>
       </c>
+      <c r="G12" t="str">
+        <v/>
+      </c>
+      <c r="H12" t="str">
+        <v/>
+      </c>
       <c r="I12" t="str">
         <v/>
       </c>
@@ -2026,6 +2089,12 @@
       <c r="F13" t="str">
         <v/>
       </c>
+      <c r="G13" t="str">
+        <v/>
+      </c>
+      <c r="H13" t="str">
+        <v/>
+      </c>
       <c r="I13" t="str">
         <v/>
       </c>
@@ -2058,6 +2127,12 @@
       <c r="F14" t="str">
         <v/>
       </c>
+      <c r="G14" t="str">
+        <v/>
+      </c>
+      <c r="H14" t="str">
+        <v/>
+      </c>
       <c r="I14" t="str">
         <v/>
       </c>
@@ -2090,6 +2165,12 @@
       <c r="F15" t="str">
         <v/>
       </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+      <c r="H15" t="str">
+        <v/>
+      </c>
       <c r="I15" t="str">
         <v/>
       </c>
@@ -2122,6 +2203,12 @@
       <c r="F16" t="str">
         <v/>
       </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+      <c r="H16" t="str">
+        <v/>
+      </c>
       <c r="I16" t="str">
         <v/>
       </c>
@@ -2154,6 +2241,12 @@
       <c r="F17" t="str">
         <v/>
       </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+      <c r="H17" t="str">
+        <v/>
+      </c>
       <c r="I17" t="str">
         <v/>
       </c>
@@ -2186,6 +2279,12 @@
       <c r="F18" t="str">
         <v/>
       </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+      <c r="H18" t="str">
+        <v/>
+      </c>
       <c r="I18" t="str">
         <v/>
       </c>
@@ -2218,6 +2317,12 @@
       <c r="F19" t="str">
         <v/>
       </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+      <c r="H19" t="str">
+        <v/>
+      </c>
       <c r="I19" t="str">
         <v/>
       </c>
@@ -2250,6 +2355,12 @@
       <c r="F20" t="str">
         <v/>
       </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+      <c r="H20" t="str">
+        <v/>
+      </c>
       <c r="I20" t="str">
         <v/>
       </c>
@@ -2282,6 +2393,12 @@
       <c r="F21" t="str">
         <v/>
       </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <v/>
+      </c>
       <c r="I21" t="str">
         <v/>
       </c>
@@ -2314,6 +2431,12 @@
       <c r="F22" t="str">
         <v/>
       </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <v/>
+      </c>
       <c r="I22" t="str">
         <v/>
       </c>
@@ -2346,6 +2469,12 @@
       <c r="F23" t="str">
         <v/>
       </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
       <c r="I23" t="str">
         <v/>
       </c>
@@ -2378,6 +2507,12 @@
       <c r="F24" t="str">
         <v/>
       </c>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+      <c r="H24" t="str">
+        <v/>
+      </c>
       <c r="I24" t="str">
         <v/>
       </c>
@@ -2410,6 +2545,12 @@
       <c r="F25" t="str">
         <v/>
       </c>
+      <c r="G25" t="str">
+        <v/>
+      </c>
+      <c r="H25" t="str">
+        <v/>
+      </c>
       <c r="I25" t="str">
         <v/>
       </c>
@@ -2442,6 +2583,12 @@
       <c r="F26" t="str">
         <v/>
       </c>
+      <c r="G26" t="str">
+        <v/>
+      </c>
+      <c r="H26" t="str">
+        <v/>
+      </c>
       <c r="I26" t="str">
         <v/>
       </c>
@@ -2474,6 +2621,12 @@
       <c r="F27" t="str">
         <v/>
       </c>
+      <c r="G27" t="str">
+        <v/>
+      </c>
+      <c r="H27" t="str">
+        <v/>
+      </c>
       <c r="I27" t="str">
         <v/>
       </c>
@@ -2506,6 +2659,12 @@
       <c r="F28" t="str">
         <v/>
       </c>
+      <c r="G28" t="str">
+        <v/>
+      </c>
+      <c r="H28" t="str">
+        <v/>
+      </c>
       <c r="I28" t="str">
         <v/>
       </c>
@@ -2538,6 +2697,12 @@
       <c r="F29" t="str">
         <v/>
       </c>
+      <c r="G29" t="str">
+        <v/>
+      </c>
+      <c r="H29" t="str">
+        <v/>
+      </c>
       <c r="I29" t="str">
         <v/>
       </c>
@@ -2570,6 +2735,12 @@
       <c r="F30" t="str">
         <v/>
       </c>
+      <c r="G30" t="str">
+        <v/>
+      </c>
+      <c r="H30" t="str">
+        <v/>
+      </c>
       <c r="I30" t="str">
         <v/>
       </c>
@@ -2602,6 +2773,12 @@
       <c r="F31" t="str">
         <v/>
       </c>
+      <c r="G31" t="str">
+        <v/>
+      </c>
+      <c r="H31" t="str">
+        <v/>
+      </c>
       <c r="I31" t="str">
         <v/>
       </c>
@@ -2634,6 +2811,12 @@
       <c r="F32" t="str">
         <v/>
       </c>
+      <c r="G32" t="str">
+        <v/>
+      </c>
+      <c r="H32" t="str">
+        <v/>
+      </c>
       <c r="I32" t="str">
         <v/>
       </c>
@@ -2666,6 +2849,12 @@
       <c r="F33" t="str">
         <v/>
       </c>
+      <c r="G33" t="str">
+        <v/>
+      </c>
+      <c r="H33" t="str">
+        <v/>
+      </c>
       <c r="I33" t="str">
         <v/>
       </c>
@@ -2698,6 +2887,12 @@
       <c r="F34" t="str">
         <v/>
       </c>
+      <c r="G34" t="str">
+        <v/>
+      </c>
+      <c r="H34" t="str">
+        <v/>
+      </c>
       <c r="I34" t="str">
         <v/>
       </c>
@@ -2730,6 +2925,12 @@
       <c r="F35" t="str">
         <v/>
       </c>
+      <c r="G35" t="str">
+        <v/>
+      </c>
+      <c r="H35" t="str">
+        <v/>
+      </c>
       <c r="I35" t="str">
         <v/>
       </c>
@@ -2762,6 +2963,12 @@
       <c r="F36" t="str">
         <v/>
       </c>
+      <c r="G36" t="str">
+        <v/>
+      </c>
+      <c r="H36" t="str">
+        <v/>
+      </c>
       <c r="I36" t="str">
         <v/>
       </c>
@@ -2794,6 +3001,12 @@
       <c r="F37" t="str">
         <v/>
       </c>
+      <c r="G37" t="str">
+        <v/>
+      </c>
+      <c r="H37" t="str">
+        <v/>
+      </c>
       <c r="I37" t="str">
         <v/>
       </c>
@@ -2826,6 +3039,12 @@
       <c r="F38" t="str">
         <v/>
       </c>
+      <c r="G38" t="str">
+        <v/>
+      </c>
+      <c r="H38" t="str">
+        <v/>
+      </c>
       <c r="I38" t="str">
         <v/>
       </c>
@@ -2858,6 +3077,12 @@
       <c r="F39" t="str">
         <v/>
       </c>
+      <c r="G39" t="str">
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <v/>
+      </c>
       <c r="I39" t="str">
         <v/>
       </c>
@@ -2890,6 +3115,12 @@
       <c r="F40" t="str">
         <v/>
       </c>
+      <c r="G40" t="str">
+        <v/>
+      </c>
+      <c r="H40" t="str">
+        <v/>
+      </c>
       <c r="I40" t="str">
         <v/>
       </c>
@@ -2922,6 +3153,12 @@
       <c r="F41" t="str">
         <v/>
       </c>
+      <c r="G41" t="str">
+        <v/>
+      </c>
+      <c r="H41" t="str">
+        <v/>
+      </c>
       <c r="I41" t="str">
         <v/>
       </c>
@@ -2954,6 +3191,12 @@
       <c r="F42" t="str">
         <v/>
       </c>
+      <c r="G42" t="str">
+        <v/>
+      </c>
+      <c r="H42" t="str">
+        <v/>
+      </c>
       <c r="I42" t="str">
         <v/>
       </c>
@@ -2986,6 +3229,12 @@
       <c r="F43" t="str">
         <v/>
       </c>
+      <c r="G43" t="str">
+        <v/>
+      </c>
+      <c r="H43" t="str">
+        <v/>
+      </c>
       <c r="I43" t="str">
         <v/>
       </c>
@@ -3018,6 +3267,12 @@
       <c r="F44" t="str">
         <v/>
       </c>
+      <c r="G44" t="str">
+        <v/>
+      </c>
+      <c r="H44" t="str">
+        <v/>
+      </c>
       <c r="I44" t="str">
         <v/>
       </c>
@@ -3050,6 +3305,12 @@
       <c r="F45" t="str">
         <v/>
       </c>
+      <c r="G45" t="str">
+        <v/>
+      </c>
+      <c r="H45" t="str">
+        <v/>
+      </c>
       <c r="I45" t="str">
         <v/>
       </c>
@@ -3082,6 +3343,12 @@
       <c r="F46" t="str">
         <v/>
       </c>
+      <c r="G46" t="str">
+        <v/>
+      </c>
+      <c r="H46" t="str">
+        <v/>
+      </c>
       <c r="I46" t="str">
         <v/>
       </c>
@@ -3114,6 +3381,12 @@
       <c r="F47" t="str">
         <v/>
       </c>
+      <c r="G47" t="str">
+        <v/>
+      </c>
+      <c r="H47" t="str">
+        <v/>
+      </c>
       <c r="I47" t="str">
         <v/>
       </c>
@@ -3146,6 +3419,12 @@
       <c r="F48" t="str">
         <v/>
       </c>
+      <c r="G48" t="str">
+        <v/>
+      </c>
+      <c r="H48" t="str">
+        <v/>
+      </c>
       <c r="I48" t="str">
         <v/>
       </c>
@@ -3178,6 +3457,12 @@
       <c r="F49" t="str">
         <v/>
       </c>
+      <c r="G49" t="str">
+        <v/>
+      </c>
+      <c r="H49" t="str">
+        <v/>
+      </c>
       <c r="I49" t="str">
         <v/>
       </c>
@@ -3210,6 +3495,12 @@
       <c r="F50" t="str">
         <v/>
       </c>
+      <c r="G50" t="str">
+        <v/>
+      </c>
+      <c r="H50" t="str">
+        <v/>
+      </c>
       <c r="I50" t="str">
         <v/>
       </c>
@@ -3242,6 +3533,12 @@
       <c r="F51" t="str">
         <v/>
       </c>
+      <c r="G51" t="str">
+        <v/>
+      </c>
+      <c r="H51" t="str">
+        <v/>
+      </c>
       <c r="I51" t="str">
         <v/>
       </c>
@@ -3274,6 +3571,12 @@
       <c r="F52" t="str">
         <v/>
       </c>
+      <c r="G52" t="str">
+        <v/>
+      </c>
+      <c r="H52" t="str">
+        <v/>
+      </c>
       <c r="I52" t="str">
         <v/>
       </c>
@@ -3306,6 +3609,12 @@
       <c r="F53" t="str">
         <v/>
       </c>
+      <c r="G53" t="str">
+        <v/>
+      </c>
+      <c r="H53" t="str">
+        <v/>
+      </c>
       <c r="I53" t="str">
         <v/>
       </c>
@@ -3338,6 +3647,12 @@
       <c r="F54" t="str">
         <v/>
       </c>
+      <c r="G54" t="str">
+        <v/>
+      </c>
+      <c r="H54" t="str">
+        <v/>
+      </c>
       <c r="I54" t="str">
         <v/>
       </c>
@@ -3370,6 +3685,12 @@
       <c r="F55" t="str">
         <v/>
       </c>
+      <c r="G55" t="str">
+        <v/>
+      </c>
+      <c r="H55" t="str">
+        <v/>
+      </c>
       <c r="I55" t="str">
         <v/>
       </c>
@@ -3402,6 +3723,12 @@
       <c r="F56" t="str">
         <v/>
       </c>
+      <c r="G56" t="str">
+        <v/>
+      </c>
+      <c r="H56" t="str">
+        <v/>
+      </c>
       <c r="I56" t="str">
         <v/>
       </c>
@@ -3434,6 +3761,12 @@
       <c r="F57" t="str">
         <v/>
       </c>
+      <c r="G57" t="str">
+        <v/>
+      </c>
+      <c r="H57" t="str">
+        <v/>
+      </c>
       <c r="I57" t="str">
         <v/>
       </c>
@@ -3466,6 +3799,12 @@
       <c r="F58" t="str">
         <v/>
       </c>
+      <c r="G58" t="str">
+        <v/>
+      </c>
+      <c r="H58" t="str">
+        <v/>
+      </c>
       <c r="I58" t="str">
         <v/>
       </c>
@@ -3498,6 +3837,12 @@
       <c r="F59" t="str">
         <v/>
       </c>
+      <c r="G59" t="str">
+        <v/>
+      </c>
+      <c r="H59" t="str">
+        <v/>
+      </c>
       <c r="I59" t="str">
         <v/>
       </c>
@@ -3530,6 +3875,12 @@
       <c r="F60" t="str">
         <v/>
       </c>
+      <c r="G60" t="str">
+        <v/>
+      </c>
+      <c r="H60" t="str">
+        <v/>
+      </c>
       <c r="I60" t="str">
         <v/>
       </c>
@@ -3562,6 +3913,12 @@
       <c r="F61" t="str">
         <v/>
       </c>
+      <c r="G61" t="str">
+        <v/>
+      </c>
+      <c r="H61" t="str">
+        <v/>
+      </c>
       <c r="I61" t="str">
         <v/>
       </c>
@@ -3594,6 +3951,12 @@
       <c r="F62" t="str">
         <v/>
       </c>
+      <c r="G62" t="str">
+        <v/>
+      </c>
+      <c r="H62" t="str">
+        <v/>
+      </c>
       <c r="I62" t="str">
         <v/>
       </c>
@@ -3626,6 +3989,12 @@
       <c r="F63" t="str">
         <v/>
       </c>
+      <c r="G63" t="str">
+        <v/>
+      </c>
+      <c r="H63" t="str">
+        <v/>
+      </c>
       <c r="I63" t="str">
         <v/>
       </c>
@@ -3658,6 +4027,12 @@
       <c r="F64" t="str">
         <v/>
       </c>
+      <c r="G64" t="str">
+        <v/>
+      </c>
+      <c r="H64" t="str">
+        <v/>
+      </c>
       <c r="I64" t="str">
         <v/>
       </c>
@@ -3690,6 +4065,12 @@
       <c r="F65" t="str">
         <v/>
       </c>
+      <c r="G65" t="str">
+        <v/>
+      </c>
+      <c r="H65" t="str">
+        <v/>
+      </c>
       <c r="I65" t="str">
         <v/>
       </c>
@@ -3722,6 +4103,12 @@
       <c r="F66" t="str">
         <v/>
       </c>
+      <c r="G66" t="str">
+        <v/>
+      </c>
+      <c r="H66" t="str">
+        <v/>
+      </c>
       <c r="I66" t="str">
         <v/>
       </c>
@@ -3754,6 +4141,12 @@
       <c r="F67" t="str">
         <v/>
       </c>
+      <c r="G67" t="str">
+        <v/>
+      </c>
+      <c r="H67" t="str">
+        <v/>
+      </c>
       <c r="I67" t="str">
         <v/>
       </c>
@@ -3786,6 +4179,12 @@
       <c r="F68" t="str">
         <v/>
       </c>
+      <c r="G68" t="str">
+        <v/>
+      </c>
+      <c r="H68" t="str">
+        <v/>
+      </c>
       <c r="I68" t="str">
         <v/>
       </c>
@@ -3818,6 +4217,12 @@
       <c r="F69" t="str">
         <v/>
       </c>
+      <c r="G69" t="str">
+        <v/>
+      </c>
+      <c r="H69" t="str">
+        <v/>
+      </c>
       <c r="I69" t="str">
         <v/>
       </c>
@@ -3850,6 +4255,12 @@
       <c r="F70" t="str">
         <v/>
       </c>
+      <c r="G70" t="str">
+        <v/>
+      </c>
+      <c r="H70" t="str">
+        <v/>
+      </c>
       <c r="I70" t="str">
         <v/>
       </c>
@@ -3882,6 +4293,12 @@
       <c r="F71" t="str">
         <v/>
       </c>
+      <c r="G71" t="str">
+        <v/>
+      </c>
+      <c r="H71" t="str">
+        <v/>
+      </c>
       <c r="I71" t="str">
         <v/>
       </c>
@@ -3914,6 +4331,12 @@
       <c r="F72" t="str">
         <v/>
       </c>
+      <c r="G72" t="str">
+        <v/>
+      </c>
+      <c r="H72" t="str">
+        <v/>
+      </c>
       <c r="I72" t="str">
         <v/>
       </c>
@@ -3946,6 +4369,12 @@
       <c r="F73" t="str">
         <v/>
       </c>
+      <c r="G73" t="str">
+        <v/>
+      </c>
+      <c r="H73" t="str">
+        <v/>
+      </c>
       <c r="I73" t="str">
         <v/>
       </c>
@@ -3978,6 +4407,12 @@
       <c r="F74" t="str">
         <v/>
       </c>
+      <c r="G74" t="str">
+        <v/>
+      </c>
+      <c r="H74" t="str">
+        <v/>
+      </c>
       <c r="I74" t="str">
         <v/>
       </c>
@@ -4010,6 +4445,12 @@
       <c r="F75" t="str">
         <v/>
       </c>
+      <c r="G75" t="str">
+        <v/>
+      </c>
+      <c r="H75" t="str">
+        <v/>
+      </c>
       <c r="I75" t="str">
         <v/>
       </c>
@@ -4042,6 +4483,12 @@
       <c r="F76" t="str">
         <v/>
       </c>
+      <c r="G76" t="str">
+        <v/>
+      </c>
+      <c r="H76" t="str">
+        <v/>
+      </c>
       <c r="I76" t="str">
         <v/>
       </c>
@@ -4074,6 +4521,12 @@
       <c r="F77" t="str">
         <v/>
       </c>
+      <c r="G77" t="str">
+        <v/>
+      </c>
+      <c r="H77" t="str">
+        <v/>
+      </c>
       <c r="I77" t="str">
         <v/>
       </c>
@@ -4106,6 +4559,12 @@
       <c r="F78" t="str">
         <v/>
       </c>
+      <c r="G78" t="str">
+        <v/>
+      </c>
+      <c r="H78" t="str">
+        <v/>
+      </c>
       <c r="I78" t="str">
         <v/>
       </c>
@@ -4138,6 +4597,12 @@
       <c r="F79" t="str">
         <v/>
       </c>
+      <c r="G79" t="str">
+        <v/>
+      </c>
+      <c r="H79" t="str">
+        <v/>
+      </c>
       <c r="I79" t="str">
         <v/>
       </c>
@@ -4170,6 +4635,12 @@
       <c r="F80" t="str">
         <v/>
       </c>
+      <c r="G80" t="str">
+        <v/>
+      </c>
+      <c r="H80" t="str">
+        <v/>
+      </c>
       <c r="I80" t="str">
         <v/>
       </c>
@@ -4202,6 +4673,12 @@
       <c r="F81" t="str">
         <v/>
       </c>
+      <c r="G81" t="str">
+        <v/>
+      </c>
+      <c r="H81" t="str">
+        <v/>
+      </c>
       <c r="I81" t="str">
         <v/>
       </c>
@@ -4234,6 +4711,12 @@
       <c r="F82" t="str">
         <v/>
       </c>
+      <c r="G82" t="str">
+        <v/>
+      </c>
+      <c r="H82" t="str">
+        <v/>
+      </c>
       <c r="I82" t="str">
         <v/>
       </c>
@@ -4266,6 +4749,12 @@
       <c r="F83" t="str">
         <v/>
       </c>
+      <c r="G83" t="str">
+        <v/>
+      </c>
+      <c r="H83" t="str">
+        <v/>
+      </c>
       <c r="I83" t="str">
         <v/>
       </c>
@@ -4298,6 +4787,12 @@
       <c r="F84" t="str">
         <v/>
       </c>
+      <c r="G84" t="str">
+        <v/>
+      </c>
+      <c r="H84" t="str">
+        <v/>
+      </c>
       <c r="I84" t="str">
         <v/>
       </c>
@@ -4330,6 +4825,12 @@
       <c r="F85" t="str">
         <v/>
       </c>
+      <c r="G85" t="str">
+        <v/>
+      </c>
+      <c r="H85" t="str">
+        <v/>
+      </c>
       <c r="I85" t="str">
         <v/>
       </c>
@@ -4362,6 +4863,12 @@
       <c r="F86" t="str">
         <v/>
       </c>
+      <c r="G86" t="str">
+        <v/>
+      </c>
+      <c r="H86" t="str">
+        <v/>
+      </c>
       <c r="I86" t="str">
         <v/>
       </c>
@@ -4394,6 +4901,12 @@
       <c r="F87" t="str">
         <v/>
       </c>
+      <c r="G87" t="str">
+        <v/>
+      </c>
+      <c r="H87" t="str">
+        <v/>
+      </c>
       <c r="I87" t="str">
         <v/>
       </c>
@@ -4426,6 +4939,12 @@
       <c r="F88" t="str">
         <v/>
       </c>
+      <c r="G88" t="str">
+        <v/>
+      </c>
+      <c r="H88" t="str">
+        <v/>
+      </c>
       <c r="I88" t="str">
         <v/>
       </c>
@@ -4458,6 +4977,12 @@
       <c r="F89" t="str">
         <v/>
       </c>
+      <c r="G89" t="str">
+        <v/>
+      </c>
+      <c r="H89" t="str">
+        <v/>
+      </c>
       <c r="I89" t="str">
         <v/>
       </c>
@@ -4490,6 +5015,12 @@
       <c r="F90" t="str">
         <v/>
       </c>
+      <c r="G90" t="str">
+        <v/>
+      </c>
+      <c r="H90" t="str">
+        <v/>
+      </c>
       <c r="I90" t="str">
         <v/>
       </c>
@@ -4522,6 +5053,12 @@
       <c r="F91" t="str">
         <v/>
       </c>
+      <c r="G91" t="str">
+        <v/>
+      </c>
+      <c r="H91" t="str">
+        <v/>
+      </c>
       <c r="I91" t="str">
         <v/>
       </c>
@@ -4554,6 +5091,12 @@
       <c r="F92" t="str">
         <v/>
       </c>
+      <c r="G92" t="str">
+        <v/>
+      </c>
+      <c r="H92" t="str">
+        <v/>
+      </c>
       <c r="I92" t="str">
         <v/>
       </c>
@@ -4586,6 +5129,12 @@
       <c r="F93" t="str">
         <v/>
       </c>
+      <c r="G93" t="str">
+        <v/>
+      </c>
+      <c r="H93" t="str">
+        <v/>
+      </c>
       <c r="I93" t="str">
         <v/>
       </c>
@@ -4618,6 +5167,12 @@
       <c r="F94" t="str">
         <v/>
       </c>
+      <c r="G94" t="str">
+        <v/>
+      </c>
+      <c r="H94" t="str">
+        <v/>
+      </c>
       <c r="I94" t="str">
         <v/>
       </c>
@@ -4650,6 +5205,12 @@
       <c r="F95" t="str">
         <v/>
       </c>
+      <c r="G95" t="str">
+        <v/>
+      </c>
+      <c r="H95" t="str">
+        <v/>
+      </c>
       <c r="I95" t="str">
         <v/>
       </c>
@@ -4682,6 +5243,12 @@
       <c r="F96" t="str">
         <v/>
       </c>
+      <c r="G96" t="str">
+        <v/>
+      </c>
+      <c r="H96" t="str">
+        <v/>
+      </c>
       <c r="I96" t="str">
         <v/>
       </c>
@@ -4714,6 +5281,12 @@
       <c r="F97" t="str">
         <v/>
       </c>
+      <c r="G97" t="str">
+        <v/>
+      </c>
+      <c r="H97" t="str">
+        <v/>
+      </c>
       <c r="I97" t="str">
         <v/>
       </c>
@@ -4746,6 +5319,12 @@
       <c r="F98" t="str">
         <v/>
       </c>
+      <c r="G98" t="str">
+        <v/>
+      </c>
+      <c r="H98" t="str">
+        <v/>
+      </c>
       <c r="I98" t="str">
         <v/>
       </c>
@@ -4778,6 +5357,12 @@
       <c r="F99" t="str">
         <v/>
       </c>
+      <c r="G99" t="str">
+        <v/>
+      </c>
+      <c r="H99" t="str">
+        <v/>
+      </c>
       <c r="I99" t="str">
         <v/>
       </c>
@@ -4810,6 +5395,12 @@
       <c r="F100" t="str">
         <v/>
       </c>
+      <c r="G100" t="str">
+        <v/>
+      </c>
+      <c r="H100" t="str">
+        <v/>
+      </c>
       <c r="I100" t="str">
         <v/>
       </c>
@@ -4842,6 +5433,12 @@
       <c r="F101" t="str">
         <v/>
       </c>
+      <c r="G101" t="str">
+        <v/>
+      </c>
+      <c r="H101" t="str">
+        <v/>
+      </c>
       <c r="I101" t="str">
         <v/>
       </c>
@@ -4874,6 +5471,12 @@
       <c r="F102" t="str">
         <v/>
       </c>
+      <c r="G102" t="str">
+        <v/>
+      </c>
+      <c r="H102" t="str">
+        <v/>
+      </c>
       <c r="I102" t="str">
         <v/>
       </c>
@@ -4906,6 +5509,12 @@
       <c r="F103" t="str">
         <v/>
       </c>
+      <c r="G103" t="str">
+        <v/>
+      </c>
+      <c r="H103" t="str">
+        <v/>
+      </c>
       <c r="I103" t="str">
         <v/>
       </c>
@@ -4938,6 +5547,12 @@
       <c r="F104" t="str">
         <v/>
       </c>
+      <c r="G104" t="str">
+        <v/>
+      </c>
+      <c r="H104" t="str">
+        <v/>
+      </c>
       <c r="I104" t="str">
         <v/>
       </c>
@@ -4970,6 +5585,12 @@
       <c r="F105" t="str">
         <v/>
       </c>
+      <c r="G105" t="str">
+        <v/>
+      </c>
+      <c r="H105" t="str">
+        <v/>
+      </c>
       <c r="I105" t="str">
         <v/>
       </c>
@@ -5002,6 +5623,12 @@
       <c r="F106" t="str">
         <v/>
       </c>
+      <c r="G106" t="str">
+        <v/>
+      </c>
+      <c r="H106" t="str">
+        <v/>
+      </c>
       <c r="I106" t="str">
         <v/>
       </c>
@@ -5034,6 +5661,12 @@
       <c r="F107" t="str">
         <v/>
       </c>
+      <c r="G107" t="str">
+        <v/>
+      </c>
+      <c r="H107" t="str">
+        <v/>
+      </c>
       <c r="I107" t="str">
         <v/>
       </c>
@@ -5066,6 +5699,12 @@
       <c r="F108" t="str">
         <v/>
       </c>
+      <c r="G108" t="str">
+        <v/>
+      </c>
+      <c r="H108" t="str">
+        <v/>
+      </c>
       <c r="I108" t="str">
         <v/>
       </c>
@@ -5098,6 +5737,12 @@
       <c r="F109" t="str">
         <v/>
       </c>
+      <c r="G109" t="str">
+        <v/>
+      </c>
+      <c r="H109" t="str">
+        <v/>
+      </c>
       <c r="I109" t="str">
         <v/>
       </c>
@@ -5130,6 +5775,12 @@
       <c r="F110" t="str">
         <v/>
       </c>
+      <c r="G110" t="str">
+        <v/>
+      </c>
+      <c r="H110" t="str">
+        <v/>
+      </c>
       <c r="I110" t="str">
         <v/>
       </c>
@@ -5162,6 +5813,12 @@
       <c r="F111" t="str">
         <v/>
       </c>
+      <c r="G111" t="str">
+        <v/>
+      </c>
+      <c r="H111" t="str">
+        <v/>
+      </c>
       <c r="I111" t="str">
         <v/>
       </c>
@@ -5194,6 +5851,12 @@
       <c r="F112" t="str">
         <v/>
       </c>
+      <c r="G112" t="str">
+        <v/>
+      </c>
+      <c r="H112" t="str">
+        <v/>
+      </c>
       <c r="I112" t="str">
         <v/>
       </c>
@@ -5226,6 +5889,12 @@
       <c r="F113" t="str">
         <v/>
       </c>
+      <c r="G113" t="str">
+        <v/>
+      </c>
+      <c r="H113" t="str">
+        <v/>
+      </c>
       <c r="I113" t="str">
         <v/>
       </c>
@@ -5258,6 +5927,12 @@
       <c r="F114" t="str">
         <v/>
       </c>
+      <c r="G114" t="str">
+        <v/>
+      </c>
+      <c r="H114" t="str">
+        <v/>
+      </c>
       <c r="I114" t="str">
         <v/>
       </c>
@@ -5290,6 +5965,12 @@
       <c r="F115" t="str">
         <v/>
       </c>
+      <c r="G115" t="str">
+        <v/>
+      </c>
+      <c r="H115" t="str">
+        <v/>
+      </c>
       <c r="I115" t="str">
         <v/>
       </c>
@@ -5322,6 +6003,12 @@
       <c r="F116" t="str">
         <v/>
       </c>
+      <c r="G116" t="str">
+        <v/>
+      </c>
+      <c r="H116" t="str">
+        <v/>
+      </c>
       <c r="I116" t="str">
         <v/>
       </c>
@@ -5354,6 +6041,12 @@
       <c r="F117" t="str">
         <v/>
       </c>
+      <c r="G117" t="str">
+        <v/>
+      </c>
+      <c r="H117" t="str">
+        <v/>
+      </c>
       <c r="I117" t="str">
         <v/>
       </c>
@@ -5386,6 +6079,12 @@
       <c r="F118" t="str">
         <v/>
       </c>
+      <c r="G118" t="str">
+        <v/>
+      </c>
+      <c r="H118" t="str">
+        <v/>
+      </c>
       <c r="I118" t="str">
         <v/>
       </c>
@@ -5418,6 +6117,12 @@
       <c r="F119" t="str">
         <v/>
       </c>
+      <c r="G119" t="str">
+        <v/>
+      </c>
+      <c r="H119" t="str">
+        <v/>
+      </c>
       <c r="I119" t="str">
         <v/>
       </c>
@@ -5450,6 +6155,12 @@
       <c r="F120" t="str">
         <v/>
       </c>
+      <c r="G120" t="str">
+        <v/>
+      </c>
+      <c r="H120" t="str">
+        <v/>
+      </c>
       <c r="I120" t="str">
         <v/>
       </c>
@@ -5482,6 +6193,12 @@
       <c r="F121" t="str">
         <v/>
       </c>
+      <c r="G121" t="str">
+        <v/>
+      </c>
+      <c r="H121" t="str">
+        <v/>
+      </c>
       <c r="I121" t="str">
         <v/>
       </c>
@@ -5514,6 +6231,12 @@
       <c r="F122" t="str">
         <v/>
       </c>
+      <c r="G122" t="str">
+        <v/>
+      </c>
+      <c r="H122" t="str">
+        <v/>
+      </c>
       <c r="I122" t="str">
         <v/>
       </c>
@@ -5546,6 +6269,12 @@
       <c r="F123" t="str">
         <v/>
       </c>
+      <c r="G123" t="str">
+        <v/>
+      </c>
+      <c r="H123" t="str">
+        <v/>
+      </c>
       <c r="I123" t="str">
         <v/>
       </c>
@@ -5578,6 +6307,12 @@
       <c r="F124" t="str">
         <v/>
       </c>
+      <c r="G124" t="str">
+        <v/>
+      </c>
+      <c r="H124" t="str">
+        <v/>
+      </c>
       <c r="I124" t="str">
         <v/>
       </c>
@@ -5610,6 +6345,12 @@
       <c r="F125" t="str">
         <v/>
       </c>
+      <c r="G125" t="str">
+        <v/>
+      </c>
+      <c r="H125" t="str">
+        <v/>
+      </c>
       <c r="I125" t="str">
         <v/>
       </c>
@@ -5642,6 +6383,12 @@
       <c r="F126" t="str">
         <v/>
       </c>
+      <c r="G126" t="str">
+        <v/>
+      </c>
+      <c r="H126" t="str">
+        <v/>
+      </c>
       <c r="I126" t="str">
         <v/>
       </c>
@@ -5674,6 +6421,12 @@
       <c r="F127" t="str">
         <v/>
       </c>
+      <c r="G127" t="str">
+        <v/>
+      </c>
+      <c r="H127" t="str">
+        <v/>
+      </c>
       <c r="I127" t="str">
         <v/>
       </c>
@@ -5706,6 +6459,12 @@
       <c r="F128" t="str">
         <v/>
       </c>
+      <c r="G128" t="str">
+        <v/>
+      </c>
+      <c r="H128" t="str">
+        <v/>
+      </c>
       <c r="I128" t="str">
         <v/>
       </c>
@@ -5738,6 +6497,12 @@
       <c r="F129" t="str">
         <v/>
       </c>
+      <c r="G129" t="str">
+        <v/>
+      </c>
+      <c r="H129" t="str">
+        <v/>
+      </c>
       <c r="I129" t="str">
         <v/>
       </c>
@@ -5770,6 +6535,12 @@
       <c r="F130" t="str">
         <v/>
       </c>
+      <c r="G130" t="str">
+        <v/>
+      </c>
+      <c r="H130" t="str">
+        <v/>
+      </c>
       <c r="I130" t="str">
         <v/>
       </c>
@@ -5802,6 +6573,12 @@
       <c r="F131" t="str">
         <v/>
       </c>
+      <c r="G131" t="str">
+        <v/>
+      </c>
+      <c r="H131" t="str">
+        <v/>
+      </c>
       <c r="I131" t="str">
         <v/>
       </c>
@@ -5834,6 +6611,12 @@
       <c r="F132" t="str">
         <v/>
       </c>
+      <c r="G132" t="str">
+        <v/>
+      </c>
+      <c r="H132" t="str">
+        <v/>
+      </c>
       <c r="I132" t="str">
         <v/>
       </c>
@@ -5866,6 +6649,12 @@
       <c r="F133" t="str">
         <v/>
       </c>
+      <c r="G133" t="str">
+        <v/>
+      </c>
+      <c r="H133" t="str">
+        <v/>
+      </c>
       <c r="I133" t="str">
         <v/>
       </c>
@@ -5898,6 +6687,12 @@
       <c r="F134" t="str">
         <v/>
       </c>
+      <c r="G134" t="str">
+        <v/>
+      </c>
+      <c r="H134" t="str">
+        <v/>
+      </c>
       <c r="I134" t="str">
         <v/>
       </c>
@@ -5930,6 +6725,12 @@
       <c r="F135" t="str">
         <v/>
       </c>
+      <c r="G135" t="str">
+        <v/>
+      </c>
+      <c r="H135" t="str">
+        <v/>
+      </c>
       <c r="I135" t="str">
         <v/>
       </c>
@@ -5962,6 +6763,12 @@
       <c r="F136" t="str">
         <v/>
       </c>
+      <c r="G136" t="str">
+        <v/>
+      </c>
+      <c r="H136" t="str">
+        <v/>
+      </c>
       <c r="I136" t="str">
         <v/>
       </c>
@@ -5994,6 +6801,12 @@
       <c r="F137" t="str">
         <v/>
       </c>
+      <c r="G137" t="str">
+        <v/>
+      </c>
+      <c r="H137" t="str">
+        <v/>
+      </c>
       <c r="I137" t="str">
         <v/>
       </c>
@@ -6026,6 +6839,12 @@
       <c r="F138" t="str">
         <v/>
       </c>
+      <c r="G138" t="str">
+        <v/>
+      </c>
+      <c r="H138" t="str">
+        <v/>
+      </c>
       <c r="I138" t="str">
         <v/>
       </c>
@@ -6058,6 +6877,12 @@
       <c r="F139" t="str">
         <v/>
       </c>
+      <c r="G139" t="str">
+        <v/>
+      </c>
+      <c r="H139" t="str">
+        <v/>
+      </c>
       <c r="I139" t="str">
         <v/>
       </c>
@@ -6090,6 +6915,12 @@
       <c r="F140" t="str">
         <v/>
       </c>
+      <c r="G140" t="str">
+        <v/>
+      </c>
+      <c r="H140" t="str">
+        <v/>
+      </c>
       <c r="I140" t="str">
         <v/>
       </c>
@@ -6122,6 +6953,12 @@
       <c r="F141" t="str">
         <v/>
       </c>
+      <c r="G141" t="str">
+        <v/>
+      </c>
+      <c r="H141" t="str">
+        <v/>
+      </c>
       <c r="I141" t="str">
         <v/>
       </c>
@@ -6154,6 +6991,12 @@
       <c r="F142" t="str">
         <v/>
       </c>
+      <c r="G142" t="str">
+        <v/>
+      </c>
+      <c r="H142" t="str">
+        <v/>
+      </c>
       <c r="I142" t="str">
         <v/>
       </c>
@@ -6186,6 +7029,12 @@
       <c r="F143" t="str">
         <v/>
       </c>
+      <c r="G143" t="str">
+        <v/>
+      </c>
+      <c r="H143" t="str">
+        <v/>
+      </c>
       <c r="I143" t="str">
         <v/>
       </c>
@@ -6218,6 +7067,12 @@
       <c r="F144" t="str">
         <v/>
       </c>
+      <c r="G144" t="str">
+        <v/>
+      </c>
+      <c r="H144" t="str">
+        <v/>
+      </c>
       <c r="I144" t="str">
         <v/>
       </c>
@@ -6250,6 +7105,12 @@
       <c r="F145" t="str">
         <v/>
       </c>
+      <c r="G145" t="str">
+        <v/>
+      </c>
+      <c r="H145" t="str">
+        <v/>
+      </c>
       <c r="I145" t="str">
         <v/>
       </c>
@@ -6282,6 +7143,12 @@
       <c r="F146" t="str">
         <v/>
       </c>
+      <c r="G146" t="str">
+        <v/>
+      </c>
+      <c r="H146" t="str">
+        <v/>
+      </c>
       <c r="I146" t="str">
         <v/>
       </c>
@@ -6314,6 +7181,12 @@
       <c r="F147" t="str">
         <v/>
       </c>
+      <c r="G147" t="str">
+        <v/>
+      </c>
+      <c r="H147" t="str">
+        <v/>
+      </c>
       <c r="I147" t="str">
         <v/>
       </c>
@@ -6346,6 +7219,12 @@
       <c r="F148" t="str">
         <v/>
       </c>
+      <c r="G148" t="str">
+        <v/>
+      </c>
+      <c r="H148" t="str">
+        <v/>
+      </c>
       <c r="I148" t="str">
         <v/>
       </c>
@@ -6378,6 +7257,12 @@
       <c r="F149" t="str">
         <v/>
       </c>
+      <c r="G149" t="str">
+        <v/>
+      </c>
+      <c r="H149" t="str">
+        <v/>
+      </c>
       <c r="I149" t="str">
         <v/>
       </c>
@@ -6410,6 +7295,12 @@
       <c r="F150" t="str">
         <v/>
       </c>
+      <c r="G150" t="str">
+        <v/>
+      </c>
+      <c r="H150" t="str">
+        <v/>
+      </c>
       <c r="I150" t="str">
         <v/>
       </c>
@@ -6442,6 +7333,12 @@
       <c r="F151" t="str">
         <v/>
       </c>
+      <c r="G151" t="str">
+        <v/>
+      </c>
+      <c r="H151" t="str">
+        <v/>
+      </c>
       <c r="I151" t="str">
         <v/>
       </c>
@@ -6474,6 +7371,12 @@
       <c r="F152" t="str">
         <v/>
       </c>
+      <c r="G152" t="str">
+        <v/>
+      </c>
+      <c r="H152" t="str">
+        <v/>
+      </c>
       <c r="I152" t="str">
         <v/>
       </c>
@@ -6506,6 +7409,12 @@
       <c r="F153" t="str">
         <v/>
       </c>
+      <c r="G153" t="str">
+        <v/>
+      </c>
+      <c r="H153" t="str">
+        <v/>
+      </c>
       <c r="I153" t="str">
         <v/>
       </c>
@@ -6538,6 +7447,12 @@
       <c r="F154" t="str">
         <v/>
       </c>
+      <c r="G154" t="str">
+        <v/>
+      </c>
+      <c r="H154" t="str">
+        <v/>
+      </c>
       <c r="I154" t="str">
         <v/>
       </c>
@@ -6570,6 +7485,12 @@
       <c r="F155" t="str">
         <v/>
       </c>
+      <c r="G155" t="str">
+        <v/>
+      </c>
+      <c r="H155" t="str">
+        <v/>
+      </c>
       <c r="I155" t="str">
         <v/>
       </c>
@@ -6602,6 +7523,12 @@
       <c r="F156" t="str">
         <v/>
       </c>
+      <c r="G156" t="str">
+        <v/>
+      </c>
+      <c r="H156" t="str">
+        <v/>
+      </c>
       <c r="I156" t="str">
         <v/>
       </c>
@@ -6634,6 +7561,12 @@
       <c r="F157" t="str">
         <v/>
       </c>
+      <c r="G157" t="str">
+        <v/>
+      </c>
+      <c r="H157" t="str">
+        <v/>
+      </c>
       <c r="I157" t="str">
         <v/>
       </c>
@@ -6666,6 +7599,12 @@
       <c r="F158" t="str">
         <v/>
       </c>
+      <c r="G158" t="str">
+        <v/>
+      </c>
+      <c r="H158" t="str">
+        <v/>
+      </c>
       <c r="I158" t="str">
         <v/>
       </c>
@@ -6698,6 +7637,12 @@
       <c r="F159" t="str">
         <v/>
       </c>
+      <c r="G159" t="str">
+        <v/>
+      </c>
+      <c r="H159" t="str">
+        <v/>
+      </c>
       <c r="I159" t="str">
         <v/>
       </c>
@@ -6730,6 +7675,12 @@
       <c r="F160" t="str">
         <v/>
       </c>
+      <c r="G160" t="str">
+        <v/>
+      </c>
+      <c r="H160" t="str">
+        <v/>
+      </c>
       <c r="I160" t="str">
         <v/>
       </c>
@@ -6762,6 +7713,12 @@
       <c r="F161" t="str">
         <v/>
       </c>
+      <c r="G161" t="str">
+        <v/>
+      </c>
+      <c r="H161" t="str">
+        <v/>
+      </c>
       <c r="I161" t="str">
         <v/>
       </c>
@@ -6794,6 +7751,12 @@
       <c r="F162" t="str">
         <v/>
       </c>
+      <c r="G162" t="str">
+        <v/>
+      </c>
+      <c r="H162" t="str">
+        <v/>
+      </c>
       <c r="I162" t="str">
         <v/>
       </c>
@@ -6826,6 +7789,12 @@
       <c r="F163" t="str">
         <v/>
       </c>
+      <c r="G163" t="str">
+        <v/>
+      </c>
+      <c r="H163" t="str">
+        <v/>
+      </c>
       <c r="I163" t="str">
         <v/>
       </c>
@@ -6858,6 +7827,12 @@
       <c r="F164" t="str">
         <v/>
       </c>
+      <c r="G164" t="str">
+        <v/>
+      </c>
+      <c r="H164" t="str">
+        <v/>
+      </c>
       <c r="I164" t="str">
         <v/>
       </c>
@@ -6890,6 +7865,12 @@
       <c r="F165" t="str">
         <v/>
       </c>
+      <c r="G165" t="str">
+        <v/>
+      </c>
+      <c r="H165" t="str">
+        <v/>
+      </c>
       <c r="I165" t="str">
         <v/>
       </c>
@@ -6922,6 +7903,12 @@
       <c r="F166" t="str">
         <v/>
       </c>
+      <c r="G166" t="str">
+        <v/>
+      </c>
+      <c r="H166" t="str">
+        <v/>
+      </c>
       <c r="I166" t="str">
         <v/>
       </c>
@@ -6954,6 +7941,12 @@
       <c r="F167" t="str">
         <v/>
       </c>
+      <c r="G167" t="str">
+        <v/>
+      </c>
+      <c r="H167" t="str">
+        <v/>
+      </c>
       <c r="I167" t="str">
         <v/>
       </c>
@@ -6986,6 +7979,12 @@
       <c r="F168" t="str">
         <v/>
       </c>
+      <c r="G168" t="str">
+        <v/>
+      </c>
+      <c r="H168" t="str">
+        <v/>
+      </c>
       <c r="I168" t="str">
         <v/>
       </c>
@@ -7018,6 +8017,12 @@
       <c r="F169" t="str">
         <v/>
       </c>
+      <c r="G169" t="str">
+        <v/>
+      </c>
+      <c r="H169" t="str">
+        <v/>
+      </c>
       <c r="I169" t="str">
         <v/>
       </c>
@@ -7050,6 +8055,12 @@
       <c r="F170" t="str">
         <v/>
       </c>
+      <c r="G170" t="str">
+        <v/>
+      </c>
+      <c r="H170" t="str">
+        <v/>
+      </c>
       <c r="I170" t="str">
         <v/>
       </c>
@@ -7082,6 +8093,12 @@
       <c r="F171" t="str">
         <v/>
       </c>
+      <c r="G171" t="str">
+        <v/>
+      </c>
+      <c r="H171" t="str">
+        <v/>
+      </c>
       <c r="I171" t="str">
         <v/>
       </c>
@@ -7114,6 +8131,12 @@
       <c r="F172" t="str">
         <v/>
       </c>
+      <c r="G172" t="str">
+        <v/>
+      </c>
+      <c r="H172" t="str">
+        <v/>
+      </c>
       <c r="I172" t="str">
         <v/>
       </c>
@@ -7146,6 +8169,12 @@
       <c r="F173" t="str">
         <v/>
       </c>
+      <c r="G173" t="str">
+        <v/>
+      </c>
+      <c r="H173" t="str">
+        <v/>
+      </c>
       <c r="I173" t="str">
         <v/>
       </c>
@@ -7178,6 +8207,12 @@
       <c r="F174" t="str">
         <v/>
       </c>
+      <c r="G174" t="str">
+        <v/>
+      </c>
+      <c r="H174" t="str">
+        <v/>
+      </c>
       <c r="I174" t="str">
         <v/>
       </c>
@@ -7210,6 +8245,12 @@
       <c r="F175" t="str">
         <v/>
       </c>
+      <c r="G175" t="str">
+        <v/>
+      </c>
+      <c r="H175" t="str">
+        <v/>
+      </c>
       <c r="I175" t="str">
         <v/>
       </c>
@@ -7242,6 +8283,12 @@
       <c r="F176" t="str">
         <v/>
       </c>
+      <c r="G176" t="str">
+        <v/>
+      </c>
+      <c r="H176" t="str">
+        <v/>
+      </c>
       <c r="I176" t="str">
         <v/>
       </c>
@@ -7274,6 +8321,12 @@
       <c r="F177" t="str">
         <v/>
       </c>
+      <c r="G177" t="str">
+        <v/>
+      </c>
+      <c r="H177" t="str">
+        <v/>
+      </c>
       <c r="I177" t="str">
         <v/>
       </c>
@@ -7306,6 +8359,12 @@
       <c r="F178" t="str">
         <v/>
       </c>
+      <c r="G178" t="str">
+        <v/>
+      </c>
+      <c r="H178" t="str">
+        <v/>
+      </c>
       <c r="I178" t="str">
         <v/>
       </c>
@@ -7338,6 +8397,12 @@
       <c r="F179" t="str">
         <v/>
       </c>
+      <c r="G179" t="str">
+        <v/>
+      </c>
+      <c r="H179" t="str">
+        <v/>
+      </c>
       <c r="I179" t="str">
         <v/>
       </c>
@@ -7370,6 +8435,12 @@
       <c r="F180" t="str">
         <v/>
       </c>
+      <c r="G180" t="str">
+        <v/>
+      </c>
+      <c r="H180" t="str">
+        <v/>
+      </c>
       <c r="I180" t="str">
         <v/>
       </c>
@@ -7402,6 +8473,12 @@
       <c r="F181" t="str">
         <v/>
       </c>
+      <c r="G181" t="str">
+        <v/>
+      </c>
+      <c r="H181" t="str">
+        <v/>
+      </c>
       <c r="I181" t="str">
         <v/>
       </c>
@@ -7434,6 +8511,12 @@
       <c r="F182" t="str">
         <v/>
       </c>
+      <c r="G182" t="str">
+        <v/>
+      </c>
+      <c r="H182" t="str">
+        <v/>
+      </c>
       <c r="I182" t="str">
         <v/>
       </c>
@@ -7466,6 +8549,12 @@
       <c r="F183" t="str">
         <v/>
       </c>
+      <c r="G183" t="str">
+        <v/>
+      </c>
+      <c r="H183" t="str">
+        <v/>
+      </c>
       <c r="I183" t="str">
         <v/>
       </c>
@@ -7498,6 +8587,12 @@
       <c r="F184" t="str">
         <v/>
       </c>
+      <c r="G184" t="str">
+        <v/>
+      </c>
+      <c r="H184" t="str">
+        <v/>
+      </c>
       <c r="I184" t="str">
         <v/>
       </c>
@@ -7530,6 +8625,12 @@
       <c r="F185" t="str">
         <v/>
       </c>
+      <c r="G185" t="str">
+        <v/>
+      </c>
+      <c r="H185" t="str">
+        <v/>
+      </c>
       <c r="I185" t="str">
         <v/>
       </c>
@@ -7562,6 +8663,12 @@
       <c r="F186" t="str">
         <v/>
       </c>
+      <c r="G186" t="str">
+        <v/>
+      </c>
+      <c r="H186" t="str">
+        <v/>
+      </c>
       <c r="I186" t="str">
         <v/>
       </c>
@@ -7594,6 +8701,12 @@
       <c r="F187" t="str">
         <v/>
       </c>
+      <c r="G187" t="str">
+        <v/>
+      </c>
+      <c r="H187" t="str">
+        <v/>
+      </c>
       <c r="I187" t="str">
         <v/>
       </c>
@@ -7626,6 +8739,12 @@
       <c r="F188" t="str">
         <v/>
       </c>
+      <c r="G188" t="str">
+        <v/>
+      </c>
+      <c r="H188" t="str">
+        <v/>
+      </c>
       <c r="I188" t="str">
         <v/>
       </c>
@@ -7658,6 +8777,12 @@
       <c r="F189" t="str">
         <v/>
       </c>
+      <c r="G189" t="str">
+        <v/>
+      </c>
+      <c r="H189" t="str">
+        <v/>
+      </c>
       <c r="I189" t="str">
         <v/>
       </c>
@@ -7690,6 +8815,12 @@
       <c r="F190" t="str">
         <v/>
       </c>
+      <c r="G190" t="str">
+        <v/>
+      </c>
+      <c r="H190" t="str">
+        <v/>
+      </c>
       <c r="I190" t="str">
         <v/>
       </c>
@@ -7722,6 +8853,12 @@
       <c r="F191" t="str">
         <v/>
       </c>
+      <c r="G191" t="str">
+        <v/>
+      </c>
+      <c r="H191" t="str">
+        <v/>
+      </c>
       <c r="I191" t="str">
         <v/>
       </c>
@@ -7754,6 +8891,12 @@
       <c r="F192" t="str">
         <v/>
       </c>
+      <c r="G192" t="str">
+        <v/>
+      </c>
+      <c r="H192" t="str">
+        <v/>
+      </c>
       <c r="I192" t="str">
         <v/>
       </c>
@@ -7786,6 +8929,12 @@
       <c r="F193" t="str">
         <v/>
       </c>
+      <c r="G193" t="str">
+        <v/>
+      </c>
+      <c r="H193" t="str">
+        <v/>
+      </c>
       <c r="I193" t="str">
         <v/>
       </c>
@@ -7818,6 +8967,12 @@
       <c r="F194" t="str">
         <v/>
       </c>
+      <c r="G194" t="str">
+        <v/>
+      </c>
+      <c r="H194" t="str">
+        <v/>
+      </c>
       <c r="I194" t="str">
         <v/>
       </c>
@@ -7850,6 +9005,12 @@
       <c r="F195" t="str">
         <v/>
       </c>
+      <c r="G195" t="str">
+        <v/>
+      </c>
+      <c r="H195" t="str">
+        <v/>
+      </c>
       <c r="I195" t="str">
         <v/>
       </c>
@@ -7882,6 +9043,12 @@
       <c r="F196" t="str">
         <v/>
       </c>
+      <c r="G196" t="str">
+        <v/>
+      </c>
+      <c r="H196" t="str">
+        <v/>
+      </c>
       <c r="I196" t="str">
         <v/>
       </c>
@@ -7914,6 +9081,12 @@
       <c r="F197" t="str">
         <v/>
       </c>
+      <c r="G197" t="str">
+        <v/>
+      </c>
+      <c r="H197" t="str">
+        <v/>
+      </c>
       <c r="I197" t="str">
         <v/>
       </c>
@@ -7946,6 +9119,12 @@
       <c r="F198" t="str">
         <v/>
       </c>
+      <c r="G198" t="str">
+        <v/>
+      </c>
+      <c r="H198" t="str">
+        <v/>
+      </c>
       <c r="I198" t="str">
         <v/>
       </c>
@@ -7978,6 +9157,12 @@
       <c r="F199" t="str">
         <v/>
       </c>
+      <c r="G199" t="str">
+        <v/>
+      </c>
+      <c r="H199" t="str">
+        <v/>
+      </c>
       <c r="I199" t="str">
         <v/>
       </c>
@@ -8010,6 +9195,12 @@
       <c r="F200" t="str">
         <v/>
       </c>
+      <c r="G200" t="str">
+        <v/>
+      </c>
+      <c r="H200" t="str">
+        <v/>
+      </c>
       <c r="I200" t="str">
         <v/>
       </c>
@@ -8042,6 +9233,12 @@
       <c r="F201" t="str">
         <v/>
       </c>
+      <c r="G201" t="str">
+        <v/>
+      </c>
+      <c r="H201" t="str">
+        <v/>
+      </c>
       <c r="I201" t="str">
         <v/>
       </c>
@@ -8074,6 +9271,12 @@
       <c r="F202" t="str">
         <v/>
       </c>
+      <c r="G202" t="str">
+        <v/>
+      </c>
+      <c r="H202" t="str">
+        <v/>
+      </c>
       <c r="I202" t="str">
         <v/>
       </c>
@@ -8106,6 +9309,12 @@
       <c r="F203" t="str">
         <v/>
       </c>
+      <c r="G203" t="str">
+        <v/>
+      </c>
+      <c r="H203" t="str">
+        <v/>
+      </c>
       <c r="I203" t="str">
         <v/>
       </c>
@@ -8138,6 +9347,12 @@
       <c r="F204" t="str">
         <v/>
       </c>
+      <c r="G204" t="str">
+        <v/>
+      </c>
+      <c r="H204" t="str">
+        <v/>
+      </c>
       <c r="I204" t="str">
         <v/>
       </c>
@@ -8170,6 +9385,12 @@
       <c r="F205" t="str">
         <v/>
       </c>
+      <c r="G205" t="str">
+        <v/>
+      </c>
+      <c r="H205" t="str">
+        <v/>
+      </c>
       <c r="I205" t="str">
         <v/>
       </c>
@@ -8202,6 +9423,12 @@
       <c r="F206" t="str">
         <v/>
       </c>
+      <c r="G206" t="str">
+        <v/>
+      </c>
+      <c r="H206" t="str">
+        <v/>
+      </c>
       <c r="I206" t="str">
         <v/>
       </c>
@@ -8234,6 +9461,12 @@
       <c r="F207" t="str">
         <v/>
       </c>
+      <c r="G207" t="str">
+        <v/>
+      </c>
+      <c r="H207" t="str">
+        <v/>
+      </c>
       <c r="I207" t="str">
         <v/>
       </c>
@@ -8266,6 +9499,12 @@
       <c r="F208" t="str">
         <v/>
       </c>
+      <c r="G208" t="str">
+        <v/>
+      </c>
+      <c r="H208" t="str">
+        <v/>
+      </c>
       <c r="I208" t="str">
         <v/>
       </c>
@@ -8298,6 +9537,12 @@
       <c r="F209" t="str">
         <v/>
       </c>
+      <c r="G209" t="str">
+        <v/>
+      </c>
+      <c r="H209" t="str">
+        <v/>
+      </c>
       <c r="I209" t="str">
         <v/>
       </c>
@@ -8330,6 +9575,12 @@
       <c r="F210" t="str">
         <v/>
       </c>
+      <c r="G210" t="str">
+        <v/>
+      </c>
+      <c r="H210" t="str">
+        <v/>
+      </c>
       <c r="I210" t="str">
         <v/>
       </c>
@@ -8362,6 +9613,12 @@
       <c r="F211" t="str">
         <v/>
       </c>
+      <c r="G211" t="str">
+        <v/>
+      </c>
+      <c r="H211" t="str">
+        <v/>
+      </c>
       <c r="I211" t="str">
         <v/>
       </c>
@@ -8394,6 +9651,12 @@
       <c r="F212" t="str">
         <v/>
       </c>
+      <c r="G212" t="str">
+        <v/>
+      </c>
+      <c r="H212" t="str">
+        <v/>
+      </c>
       <c r="I212" t="str">
         <v/>
       </c>
@@ -8426,6 +9689,12 @@
       <c r="F213" t="str">
         <v/>
       </c>
+      <c r="G213" t="str">
+        <v/>
+      </c>
+      <c r="H213" t="str">
+        <v/>
+      </c>
       <c r="I213" t="str">
         <v/>
       </c>
@@ -8458,6 +9727,12 @@
       <c r="F214" t="str">
         <v/>
       </c>
+      <c r="G214" t="str">
+        <v/>
+      </c>
+      <c r="H214" t="str">
+        <v/>
+      </c>
       <c r="I214" t="str">
         <v/>
       </c>
@@ -8490,6 +9765,12 @@
       <c r="F215" t="str">
         <v/>
       </c>
+      <c r="G215" t="str">
+        <v/>
+      </c>
+      <c r="H215" t="str">
+        <v/>
+      </c>
       <c r="I215" t="str">
         <v/>
       </c>
@@ -8522,6 +9803,12 @@
       <c r="F216" t="str">
         <v/>
       </c>
+      <c r="G216" t="str">
+        <v/>
+      </c>
+      <c r="H216" t="str">
+        <v/>
+      </c>
       <c r="I216" t="str">
         <v/>
       </c>
@@ -8554,6 +9841,12 @@
       <c r="F217" t="str">
         <v/>
       </c>
+      <c r="G217" t="str">
+        <v/>
+      </c>
+      <c r="H217" t="str">
+        <v/>
+      </c>
       <c r="I217" t="str">
         <v/>
       </c>
@@ -8586,6 +9879,12 @@
       <c r="F218" t="str">
         <v/>
       </c>
+      <c r="G218" t="str">
+        <v/>
+      </c>
+      <c r="H218" t="str">
+        <v/>
+      </c>
       <c r="I218" t="str">
         <v/>
       </c>
@@ -8618,6 +9917,12 @@
       <c r="F219" t="str">
         <v/>
       </c>
+      <c r="G219" t="str">
+        <v/>
+      </c>
+      <c r="H219" t="str">
+        <v/>
+      </c>
       <c r="I219" t="str">
         <v/>
       </c>
@@ -8650,6 +9955,12 @@
       <c r="F220" t="str">
         <v/>
       </c>
+      <c r="G220" t="str">
+        <v/>
+      </c>
+      <c r="H220" t="str">
+        <v/>
+      </c>
       <c r="I220" t="str">
         <v/>
       </c>
@@ -8682,6 +9993,12 @@
       <c r="F221" t="str">
         <v/>
       </c>
+      <c r="G221" t="str">
+        <v/>
+      </c>
+      <c r="H221" t="str">
+        <v/>
+      </c>
       <c r="I221" t="str">
         <v/>
       </c>
@@ -8714,6 +10031,12 @@
       <c r="F222" t="str">
         <v/>
       </c>
+      <c r="G222" t="str">
+        <v/>
+      </c>
+      <c r="H222" t="str">
+        <v/>
+      </c>
       <c r="I222" t="str">
         <v/>
       </c>
@@ -8746,6 +10069,12 @@
       <c r="F223" t="str">
         <v/>
       </c>
+      <c r="G223" t="str">
+        <v/>
+      </c>
+      <c r="H223" t="str">
+        <v/>
+      </c>
       <c r="I223" t="str">
         <v/>
       </c>
@@ -8778,6 +10107,12 @@
       <c r="F224" t="str">
         <v/>
       </c>
+      <c r="G224" t="str">
+        <v/>
+      </c>
+      <c r="H224" t="str">
+        <v/>
+      </c>
       <c r="I224" t="str">
         <v/>
       </c>
@@ -8810,6 +10145,12 @@
       <c r="F225" t="str">
         <v/>
       </c>
+      <c r="G225" t="str">
+        <v/>
+      </c>
+      <c r="H225" t="str">
+        <v/>
+      </c>
       <c r="I225" t="str">
         <v/>
       </c>
@@ -8842,6 +10183,12 @@
       <c r="F226" t="str">
         <v/>
       </c>
+      <c r="G226" t="str">
+        <v/>
+      </c>
+      <c r="H226" t="str">
+        <v/>
+      </c>
       <c r="I226" t="str">
         <v/>
       </c>
@@ -8874,6 +10221,12 @@
       <c r="F227" t="str">
         <v/>
       </c>
+      <c r="G227" t="str">
+        <v/>
+      </c>
+      <c r="H227" t="str">
+        <v/>
+      </c>
       <c r="I227" t="str">
         <v/>
       </c>
@@ -8906,6 +10259,12 @@
       <c r="F228" t="str">
         <v/>
       </c>
+      <c r="G228" t="str">
+        <v/>
+      </c>
+      <c r="H228" t="str">
+        <v/>
+      </c>
       <c r="I228" t="str">
         <v/>
       </c>
@@ -8938,6 +10297,12 @@
       <c r="F229" t="str">
         <v/>
       </c>
+      <c r="G229" t="str">
+        <v/>
+      </c>
+      <c r="H229" t="str">
+        <v/>
+      </c>
       <c r="I229" t="str">
         <v/>
       </c>
@@ -8970,6 +10335,12 @@
       <c r="F230" t="str">
         <v/>
       </c>
+      <c r="G230" t="str">
+        <v/>
+      </c>
+      <c r="H230" t="str">
+        <v/>
+      </c>
       <c r="I230" t="str">
         <v/>
       </c>
@@ -9002,6 +10373,12 @@
       <c r="F231" t="str">
         <v/>
       </c>
+      <c r="G231" t="str">
+        <v/>
+      </c>
+      <c r="H231" t="str">
+        <v/>
+      </c>
       <c r="I231" t="str">
         <v/>
       </c>
@@ -9034,6 +10411,12 @@
       <c r="F232" t="str">
         <v/>
       </c>
+      <c r="G232" t="str">
+        <v/>
+      </c>
+      <c r="H232" t="str">
+        <v/>
+      </c>
       <c r="I232" t="str">
         <v/>
       </c>
@@ -9066,6 +10449,12 @@
       <c r="F233" t="str">
         <v/>
       </c>
+      <c r="G233" t="str">
+        <v/>
+      </c>
+      <c r="H233" t="str">
+        <v/>
+      </c>
       <c r="I233" t="str">
         <v/>
       </c>
@@ -9098,6 +10487,12 @@
       <c r="F234" t="str">
         <v/>
       </c>
+      <c r="G234" t="str">
+        <v/>
+      </c>
+      <c r="H234" t="str">
+        <v/>
+      </c>
       <c r="I234" t="str">
         <v/>
       </c>
@@ -9130,6 +10525,12 @@
       <c r="F235" t="str">
         <v/>
       </c>
+      <c r="G235" t="str">
+        <v/>
+      </c>
+      <c r="H235" t="str">
+        <v/>
+      </c>
       <c r="I235" t="str">
         <v/>
       </c>
@@ -9162,6 +10563,12 @@
       <c r="F236" t="str">
         <v/>
       </c>
+      <c r="G236" t="str">
+        <v/>
+      </c>
+      <c r="H236" t="str">
+        <v/>
+      </c>
       <c r="I236" t="str">
         <v/>
       </c>
@@ -9194,6 +10601,12 @@
       <c r="F237" t="str">
         <v/>
       </c>
+      <c r="G237" t="str">
+        <v/>
+      </c>
+      <c r="H237" t="str">
+        <v/>
+      </c>
       <c r="I237" t="str">
         <v/>
       </c>
@@ -9226,6 +10639,12 @@
       <c r="F238" t="str">
         <v/>
       </c>
+      <c r="G238" t="str">
+        <v/>
+      </c>
+      <c r="H238" t="str">
+        <v/>
+      </c>
       <c r="I238" t="str">
         <v/>
       </c>
@@ -9258,6 +10677,12 @@
       <c r="F239" t="str">
         <v/>
       </c>
+      <c r="G239" t="str">
+        <v/>
+      </c>
+      <c r="H239" t="str">
+        <v/>
+      </c>
       <c r="I239" t="str">
         <v/>
       </c>
@@ -9290,6 +10715,12 @@
       <c r="F240" t="str">
         <v/>
       </c>
+      <c r="G240" t="str">
+        <v/>
+      </c>
+      <c r="H240" t="str">
+        <v/>
+      </c>
       <c r="I240" t="str">
         <v/>
       </c>
@@ -9322,6 +10753,12 @@
       <c r="F241" t="str">
         <v/>
       </c>
+      <c r="G241" t="str">
+        <v/>
+      </c>
+      <c r="H241" t="str">
+        <v/>
+      </c>
       <c r="I241" t="str">
         <v/>
       </c>
@@ -9354,6 +10791,12 @@
       <c r="F242" t="str">
         <v/>
       </c>
+      <c r="G242" t="str">
+        <v/>
+      </c>
+      <c r="H242" t="str">
+        <v/>
+      </c>
       <c r="I242" t="str">
         <v/>
       </c>
@@ -9386,6 +10829,12 @@
       <c r="F243" t="str">
         <v/>
       </c>
+      <c r="G243" t="str">
+        <v/>
+      </c>
+      <c r="H243" t="str">
+        <v/>
+      </c>
       <c r="I243" t="str">
         <v/>
       </c>
@@ -9418,6 +10867,12 @@
       <c r="F244" t="str">
         <v/>
       </c>
+      <c r="G244" t="str">
+        <v/>
+      </c>
+      <c r="H244" t="str">
+        <v/>
+      </c>
       <c r="I244" t="str">
         <v/>
       </c>
@@ -9450,6 +10905,12 @@
       <c r="F245" t="str">
         <v/>
       </c>
+      <c r="G245" t="str">
+        <v/>
+      </c>
+      <c r="H245" t="str">
+        <v/>
+      </c>
       <c r="I245" t="str">
         <v/>
       </c>
@@ -9482,6 +10943,12 @@
       <c r="F246" t="str">
         <v/>
       </c>
+      <c r="G246" t="str">
+        <v/>
+      </c>
+      <c r="H246" t="str">
+        <v/>
+      </c>
       <c r="I246" t="str">
         <v/>
       </c>
@@ -9514,6 +10981,12 @@
       <c r="F247" t="str">
         <v/>
       </c>
+      <c r="G247" t="str">
+        <v/>
+      </c>
+      <c r="H247" t="str">
+        <v/>
+      </c>
       <c r="I247" t="str">
         <v/>
       </c>
@@ -9546,6 +11019,12 @@
       <c r="F248" t="str">
         <v/>
       </c>
+      <c r="G248" t="str">
+        <v/>
+      </c>
+      <c r="H248" t="str">
+        <v/>
+      </c>
       <c r="I248" t="str">
         <v/>
       </c>
@@ -9578,6 +11057,12 @@
       <c r="F249" t="str">
         <v/>
       </c>
+      <c r="G249" t="str">
+        <v/>
+      </c>
+      <c r="H249" t="str">
+        <v/>
+      </c>
       <c r="I249" t="str">
         <v/>
       </c>
@@ -9610,6 +11095,12 @@
       <c r="F250" t="str">
         <v/>
       </c>
+      <c r="G250" t="str">
+        <v/>
+      </c>
+      <c r="H250" t="str">
+        <v/>
+      </c>
       <c r="I250" t="str">
         <v/>
       </c>
@@ -9642,6 +11133,12 @@
       <c r="F251" t="str">
         <v/>
       </c>
+      <c r="G251" t="str">
+        <v/>
+      </c>
+      <c r="H251" t="str">
+        <v/>
+      </c>
       <c r="I251" t="str">
         <v/>
       </c>
@@ -9674,6 +11171,12 @@
       <c r="F252" t="str">
         <v/>
       </c>
+      <c r="G252" t="str">
+        <v/>
+      </c>
+      <c r="H252" t="str">
+        <v/>
+      </c>
       <c r="I252" t="str">
         <v/>
       </c>
@@ -9706,6 +11209,12 @@
       <c r="F253" t="str">
         <v/>
       </c>
+      <c r="G253" t="str">
+        <v/>
+      </c>
+      <c r="H253" t="str">
+        <v/>
+      </c>
       <c r="I253" t="str">
         <v/>
       </c>
@@ -9738,6 +11247,12 @@
       <c r="F254" t="str">
         <v/>
       </c>
+      <c r="G254" t="str">
+        <v/>
+      </c>
+      <c r="H254" t="str">
+        <v/>
+      </c>
       <c r="I254" t="str">
         <v/>
       </c>
@@ -9770,6 +11285,12 @@
       <c r="F255" t="str">
         <v/>
       </c>
+      <c r="G255" t="str">
+        <v/>
+      </c>
+      <c r="H255" t="str">
+        <v/>
+      </c>
       <c r="I255" t="str">
         <v/>
       </c>
@@ -9802,6 +11323,12 @@
       <c r="F256" t="str">
         <v/>
       </c>
+      <c r="G256" t="str">
+        <v/>
+      </c>
+      <c r="H256" t="str">
+        <v/>
+      </c>
       <c r="I256" t="str">
         <v/>
       </c>
@@ -9832,6 +11359,12 @@
         <v>Hand Cash</v>
       </c>
       <c r="F257" t="str">
+        <v/>
+      </c>
+      <c r="G257" t="str">
+        <v/>
+      </c>
+      <c r="H257" t="str">
         <v/>
       </c>
       <c r="I257" t="str">

</xml_diff>

<commit_message>
Enhanced index.html by adding family member filtering and export functionality for filtered data to Excel and image formats. Updated language support for family member options in multiple languages. Updated finance_data.xlsx for compatibility with these new features.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -598,7 +598,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -669,6 +669,9 @@
       <c r="H2" t="str">
         <v>equal</v>
       </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
       <c r="J2" t="str">
         <v/>
       </c>
@@ -682,9 +685,44 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>bazar</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Ammu</v>
+      </c>
+      <c r="C3">
+        <v>9.99</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2025-12-28</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Hand Cash</v>
+      </c>
+      <c r="G3" t="str">
+        <v>["me"]</v>
+      </c>
+      <c r="H3" t="str">
+        <v>equal</v>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L3" t="str">
+        <v/>
+      </c>
+      <c r="M3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added support for debts in state management and Excel export functionality in index.html, enhancing financial tracking capabilities.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Accounts" sheetId="9" r:id="rId9"/>
     <sheet name="Transfers" sheetId="10" r:id="rId10"/>
     <sheet name="FamilyMembers" sheetId="11" r:id="rId11"/>
+    <sheet name="Debts" sheetId="12" r:id="rId12"/>
   </sheets>
 </workbook>
 </file>
@@ -596,6 +597,66 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>type</v>
+      </c>
+      <c r="C1" t="str">
+        <v>principal</v>
+      </c>
+      <c r="D1" t="str">
+        <v>paid</v>
+      </c>
+      <c r="E1" t="str">
+        <v>creditor</v>
+      </c>
+      <c r="F1" t="str">
+        <v>dueDate</v>
+      </c>
+      <c r="G1" t="str">
+        <v>description</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>HOme</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Loan</v>
+      </c>
+      <c r="C2">
+        <v>50000</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v>2026-01-02</v>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M3"/>
@@ -701,11 +762,17 @@
       <c r="E3" t="str">
         <v>Hand Cash</v>
       </c>
+      <c r="F3" t="str">
+        <v/>
+      </c>
       <c r="G3" t="str">
         <v>["me"]</v>
       </c>
       <c r="H3" t="str">
         <v>equal</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
       </c>
       <c r="J3" t="str">
         <v/>

</xml_diff>

<commit_message>
Add styles for payment history and Islamic properties summary
- Introduced grid layout for payment history summary and items.
- Styled payment history components including labels, values, and notes.
- Added styles for properties and Islamic cards with responsive design.
- Enhanced visual appearance with background gradients and shadows.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -15,6 +15,8 @@
     <sheet name="Transfers" sheetId="10" r:id="rId10"/>
     <sheet name="FamilyMembers" sheetId="11" r:id="rId11"/>
     <sheet name="Debts" sheetId="12" r:id="rId12"/>
+    <sheet name="Properties" sheetId="13" r:id="rId13"/>
+    <sheet name="Islamic" sheetId="14" r:id="rId14"/>
   </sheets>
 </workbook>
 </file>
@@ -599,7 +601,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -615,16 +617,22 @@
         <v>principal</v>
       </c>
       <c r="D1" t="str">
+        <v>paymentHistory</v>
+      </c>
+      <c r="E1" t="str">
+        <v>historicalPaid</v>
+      </c>
+      <c r="F1" t="str">
+        <v>creditor</v>
+      </c>
+      <c r="G1" t="str">
+        <v>dueDate</v>
+      </c>
+      <c r="H1" t="str">
+        <v>description</v>
+      </c>
+      <c r="I1" t="str">
         <v>paid</v>
-      </c>
-      <c r="E1" t="str">
-        <v>creditor</v>
-      </c>
-      <c r="F1" t="str">
-        <v>dueDate</v>
-      </c>
-      <c r="G1" t="str">
-        <v>description</v>
       </c>
     </row>
     <row r="2">
@@ -637,29 +645,120 @@
       <c r="C2">
         <v>50000</v>
       </c>
+      <c r="D2" t="str">
+        <v>[{"amount":5000,"date":"2026-01-02","note":"","method":"Cash","recordedAt":"2026-01-02T06:58:03.990Z"}]</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v>2026-01-02</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2">
+        <v>5000</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>type</v>
+      </c>
+      <c r="C1" t="str">
+        <v>value</v>
+      </c>
+      <c r="D1" t="str">
+        <v>estimatedValue</v>
+      </c>
+      <c r="E1" t="str">
+        <v>location</v>
+      </c>
+      <c r="F1" t="str">
+        <v>area</v>
+      </c>
+      <c r="G1" t="str">
+        <v>acquiredDate</v>
+      </c>
+      <c r="H1" t="str">
+        <v>zakatEligible</v>
+      </c>
+      <c r="I1" t="str">
+        <v>notes</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>gold</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Gold</v>
+      </c>
+      <c r="C2">
+        <v>50000</v>
+      </c>
       <c r="D2">
-        <v>0</v>
+        <v>50000</v>
       </c>
       <c r="E2" t="str">
         <v/>
       </c>
-      <c r="F2" t="str">
-        <v>2026-01-02</v>
+      <c r="F2">
+        <v>-0.01</v>
       </c>
       <c r="G2" t="str">
+        <v>2026-01-01</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -737,13 +836,13 @@
         <v/>
       </c>
       <c r="K2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L2" t="str">
-        <v/>
+        <v>monthly</v>
       </c>
       <c r="M2" t="str">
-        <v/>
+        <v>2026-01-31</v>
       </c>
     </row>
     <row r="3">
@@ -787,9 +886,50 @@
         <v/>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>office ar chele</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Other</v>
+      </c>
+      <c r="C4">
+        <v>5000</v>
+      </c>
+      <c r="D4" t="str">
+        <v>2026-01-01</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Hand Cash</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Husna</v>
+      </c>
+      <c r="G4" t="str">
+        <v>["vaiya","me"]</v>
+      </c>
+      <c r="H4" t="str">
+        <v>equal</v>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="str">
+        <v>monthly</v>
+      </c>
+      <c r="M4" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M4"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Enhance index.html with equation evaluation and display for input fields
- Added functionality to evaluate mathematical equations entered in input fields.
- Implemented a display for the result of equations, improving user interaction.
- Updated number parsing to preserve equation strings while normalizing numeric values.
- Enhanced balance calculations to utilize the new parsing logic for improved accuracy.
- Updated finance_data.xlsx to ensure compatibility with the new features.
</commit_message>
<xml_diff>
--- a/finance_data.xlsx
+++ b/finance_data.xlsx
@@ -410,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -485,9 +485,41 @@
         <v/>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Giant Marketers</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Salary</v>
+      </c>
+      <c r="C3" t="str">
+        <v>25000+5000</v>
+      </c>
+      <c r="D3" t="str">
+        <v>2026-02-01</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Dutch Bangla Bank</v>
+      </c>
+      <c r="F3" t="str">
+        <v>me</v>
+      </c>
+      <c r="G3" t="str">
+        <v/>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>